<commit_message>
Added Server profiling of number of threads and organized folders
</commit_message>
<xml_diff>
--- a/Profiling OMP/DHPC.xlsx
+++ b/Profiling OMP/DHPC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francisco Câmara\OneDrive\Ambiente de Trabalho\DHPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B1FD80-71C3-43DE-9693-38E3C0A3A369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058C2457-A023-44D0-B287-5598C8DE9CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
   <si>
     <t>Scheduling Type</t>
   </si>
@@ -79,7 +79,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,8 +93,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,8 +125,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="45">
+  <borders count="55">
     <border>
       <left/>
       <right/>
@@ -682,11 +694,137 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -766,10 +904,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -784,93 +958,98 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1151,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AT22"/>
+  <dimension ref="B2:BB48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="V14" workbookViewId="0">
+      <selection activeCell="AK37" sqref="AK37:AN41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,190 +1341,206 @@
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="E3" s="50" t="s">
+    <row r="2" spans="2:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:50" x14ac:dyDescent="0.25">
+      <c r="E3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="51"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="51"/>
-      <c r="U3" s="51"/>
-      <c r="V3" s="51"/>
-      <c r="W3" s="51"/>
-      <c r="X3" s="51"/>
-      <c r="Y3" s="51"/>
-      <c r="Z3" s="51"/>
-      <c r="AA3" s="51"/>
-      <c r="AB3" s="51"/>
-      <c r="AC3" s="51"/>
-      <c r="AD3" s="51"/>
-      <c r="AE3" s="51"/>
-      <c r="AF3" s="51"/>
-      <c r="AG3" s="51"/>
-      <c r="AH3" s="51"/>
-      <c r="AI3" s="51"/>
-      <c r="AJ3" s="51"/>
-      <c r="AK3" s="51"/>
-      <c r="AL3" s="52"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="35"/>
+      <c r="V3" s="35"/>
+      <c r="W3" s="35"/>
+      <c r="X3" s="35"/>
+      <c r="Y3" s="35"/>
+      <c r="Z3" s="35"/>
+      <c r="AA3" s="35"/>
+      <c r="AB3" s="35"/>
+      <c r="AC3" s="35"/>
+      <c r="AD3" s="35"/>
+      <c r="AE3" s="35"/>
+      <c r="AF3" s="35"/>
+      <c r="AG3" s="35"/>
+      <c r="AH3" s="35"/>
+      <c r="AI3" s="35"/>
+      <c r="AJ3" s="35"/>
+      <c r="AK3" s="35"/>
+      <c r="AL3" s="35"/>
+      <c r="AM3" s="35"/>
+      <c r="AN3" s="35"/>
+      <c r="AO3" s="35"/>
+      <c r="AP3" s="36"/>
     </row>
-    <row r="4" spans="2:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="53"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
-      <c r="O4" s="54"/>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="54"/>
-      <c r="S4" s="54"/>
-      <c r="T4" s="54"/>
-      <c r="U4" s="54"/>
-      <c r="V4" s="54"/>
-      <c r="W4" s="54"/>
-      <c r="X4" s="54"/>
-      <c r="Y4" s="54"/>
-      <c r="Z4" s="54"/>
-      <c r="AA4" s="54"/>
-      <c r="AB4" s="54"/>
-      <c r="AC4" s="54"/>
-      <c r="AD4" s="54"/>
-      <c r="AE4" s="54"/>
-      <c r="AF4" s="54"/>
-      <c r="AG4" s="54"/>
-      <c r="AH4" s="54"/>
-      <c r="AI4" s="54"/>
-      <c r="AJ4" s="54"/>
-      <c r="AK4" s="54"/>
-      <c r="AL4" s="55"/>
+    <row r="4" spans="2:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="37"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="38"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="38"/>
+      <c r="W4" s="38"/>
+      <c r="X4" s="38"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="38"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="38"/>
+      <c r="AG4" s="38"/>
+      <c r="AH4" s="38"/>
+      <c r="AI4" s="38"/>
+      <c r="AJ4" s="38"/>
+      <c r="AK4" s="38"/>
+      <c r="AL4" s="38"/>
+      <c r="AM4" s="38"/>
+      <c r="AN4" s="38"/>
+      <c r="AO4" s="38"/>
+      <c r="AP4" s="39"/>
     </row>
-    <row r="5" spans="2:46" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="44" t="s">
+    <row r="5" spans="2:50" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="50" t="s">
+      <c r="D5" s="53"/>
+      <c r="E5" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="50" t="s">
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="51"/>
-      <c r="R5" s="51"/>
-      <c r="S5" s="51"/>
-      <c r="T5" s="51"/>
-      <c r="U5" s="51"/>
-      <c r="V5" s="51"/>
-      <c r="W5" s="51"/>
-      <c r="X5" s="51"/>
-      <c r="Y5" s="51"/>
-      <c r="Z5" s="52"/>
-      <c r="AA5" s="50" t="s">
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="35"/>
+      <c r="V5" s="35"/>
+      <c r="W5" s="35"/>
+      <c r="X5" s="35"/>
+      <c r="Y5" s="35"/>
+      <c r="Z5" s="36"/>
+      <c r="AA5" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AB5" s="51"/>
-      <c r="AC5" s="51"/>
-      <c r="AD5" s="51"/>
-      <c r="AE5" s="51"/>
-      <c r="AF5" s="51"/>
-      <c r="AG5" s="51"/>
-      <c r="AH5" s="51"/>
-      <c r="AI5" s="51"/>
-      <c r="AJ5" s="51"/>
-      <c r="AK5" s="52"/>
-      <c r="AL5" s="40" t="s">
+      <c r="AB5" s="35"/>
+      <c r="AC5" s="35"/>
+      <c r="AD5" s="35"/>
+      <c r="AE5" s="35"/>
+      <c r="AF5" s="35"/>
+      <c r="AG5" s="35"/>
+      <c r="AH5" s="35"/>
+      <c r="AI5" s="35"/>
+      <c r="AJ5" s="35"/>
+      <c r="AK5" s="36"/>
+      <c r="AL5" s="29"/>
+      <c r="AM5" s="29"/>
+      <c r="AN5" s="29"/>
+      <c r="AO5" s="29"/>
+      <c r="AP5" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="AM5" s="40" t="s">
+      <c r="AQ5" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="AN5" s="15"/>
-      <c r="AO5" s="15"/>
-      <c r="AP5" s="15"/>
-      <c r="AQ5" s="15"/>
       <c r="AR5" s="15"/>
       <c r="AS5" s="15"/>
       <c r="AT5" s="15"/>
+      <c r="AU5" s="15"/>
+      <c r="AV5" s="15"/>
+      <c r="AW5" s="15"/>
+      <c r="AX5" s="15"/>
     </row>
-    <row r="6" spans="2:46" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="46"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="55"/>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="54"/>
-      <c r="R6" s="54"/>
-      <c r="S6" s="54"/>
-      <c r="T6" s="54"/>
-      <c r="U6" s="54"/>
-      <c r="V6" s="54"/>
-      <c r="W6" s="54"/>
-      <c r="X6" s="54"/>
-      <c r="Y6" s="54"/>
-      <c r="Z6" s="55"/>
-      <c r="AA6" s="53"/>
-      <c r="AB6" s="54"/>
-      <c r="AC6" s="54"/>
-      <c r="AD6" s="54"/>
-      <c r="AE6" s="54"/>
-      <c r="AF6" s="54"/>
-      <c r="AG6" s="54"/>
-      <c r="AH6" s="54"/>
-      <c r="AI6" s="54"/>
-      <c r="AJ6" s="54"/>
-      <c r="AK6" s="55"/>
-      <c r="AL6" s="56"/>
-      <c r="AM6" s="41"/>
-      <c r="AN6" s="15"/>
-      <c r="AO6" s="15"/>
-      <c r="AP6" s="15"/>
-      <c r="AQ6" s="15"/>
+    <row r="6" spans="2:50" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="54"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="38"/>
+      <c r="T6" s="38"/>
+      <c r="U6" s="38"/>
+      <c r="V6" s="38"/>
+      <c r="W6" s="38"/>
+      <c r="X6" s="38"/>
+      <c r="Y6" s="38"/>
+      <c r="Z6" s="39"/>
+      <c r="AA6" s="37"/>
+      <c r="AB6" s="38"/>
+      <c r="AC6" s="38"/>
+      <c r="AD6" s="38"/>
+      <c r="AE6" s="38"/>
+      <c r="AF6" s="38"/>
+      <c r="AG6" s="38"/>
+      <c r="AH6" s="38"/>
+      <c r="AI6" s="38"/>
+      <c r="AJ6" s="38"/>
+      <c r="AK6" s="39"/>
+      <c r="AL6" s="30"/>
+      <c r="AM6" s="30"/>
+      <c r="AN6" s="30"/>
+      <c r="AO6" s="30"/>
+      <c r="AP6" s="60"/>
+      <c r="AQ6" s="44"/>
       <c r="AR6" s="15"/>
       <c r="AS6" s="15"/>
       <c r="AT6" s="15"/>
+      <c r="AU6" s="15"/>
+      <c r="AV6" s="15"/>
+      <c r="AW6" s="15"/>
+      <c r="AX6" s="15"/>
     </row>
-    <row r="7" spans="2:46" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="29" t="s">
+    <row r="7" spans="2:50" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="48"/>
+      <c r="D7" s="57"/>
       <c r="E7" s="2">
         <v>1</v>
       </c>
@@ -1445,21 +1640,25 @@
       <c r="AK7" s="3">
         <v>1000</v>
       </c>
-      <c r="AL7" s="22" t="s">
+      <c r="AL7" s="77"/>
+      <c r="AM7" s="77"/>
+      <c r="AN7" s="77"/>
+      <c r="AO7" s="77"/>
+      <c r="AP7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="AM7" s="18" t="s">
+      <c r="AQ7" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:46" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="31" t="s">
+    <row r="8" spans="2:50" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="42"/>
+      <c r="D8" s="49"/>
       <c r="E8" s="11">
         <v>7398</v>
       </c>
@@ -1559,19 +1758,23 @@
       <c r="AK8" s="13">
         <v>12719</v>
       </c>
-      <c r="AL8" s="23">
+      <c r="AL8" s="78"/>
+      <c r="AM8" s="78"/>
+      <c r="AN8" s="78"/>
+      <c r="AO8" s="78"/>
+      <c r="AP8" s="23">
         <v>14986</v>
       </c>
-      <c r="AM8" s="19">
+      <c r="AQ8" s="19">
         <v>48421</v>
       </c>
     </row>
-    <row r="9" spans="2:46" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="32"/>
-      <c r="C9" s="36" t="s">
+    <row r="9" spans="2:50" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="46"/>
+      <c r="C9" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="49"/>
+      <c r="D9" s="59"/>
       <c r="E9" s="4">
         <v>4144</v>
       </c>
@@ -1671,19 +1874,23 @@
       <c r="AK9" s="5">
         <v>7495</v>
       </c>
-      <c r="AL9" s="24">
+      <c r="AL9" s="79"/>
+      <c r="AM9" s="79"/>
+      <c r="AN9" s="79"/>
+      <c r="AO9" s="79"/>
+      <c r="AP9" s="24">
         <v>9367</v>
       </c>
-      <c r="AM9" s="20">
+      <c r="AQ9" s="20">
         <v>26219</v>
       </c>
     </row>
-    <row r="10" spans="2:46" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="32"/>
-      <c r="C10" s="34" t="s">
+    <row r="10" spans="2:50" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="46"/>
+      <c r="C10" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="42"/>
+      <c r="D10" s="49"/>
       <c r="E10" s="4">
         <v>2385</v>
       </c>
@@ -1783,19 +1990,23 @@
       <c r="AK10" s="5">
         <v>6304</v>
       </c>
-      <c r="AL10" s="24">
+      <c r="AL10" s="79"/>
+      <c r="AM10" s="79"/>
+      <c r="AN10" s="79"/>
+      <c r="AO10" s="79"/>
+      <c r="AP10" s="24">
         <v>5364</v>
       </c>
-      <c r="AM10" s="20">
+      <c r="AQ10" s="20">
         <v>15398</v>
       </c>
     </row>
-    <row r="11" spans="2:46" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="33"/>
-      <c r="C11" s="38" t="s">
+    <row r="11" spans="2:50" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="47"/>
+      <c r="C11" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="43"/>
+      <c r="D11" s="51"/>
       <c r="E11" s="6">
         <v>180093</v>
       </c>
@@ -1895,54 +2106,58 @@
       <c r="AK11" s="8">
         <v>274438</v>
       </c>
-      <c r="AL11" s="25">
+      <c r="AL11" s="80"/>
+      <c r="AM11" s="80"/>
+      <c r="AN11" s="80"/>
+      <c r="AO11" s="80"/>
+      <c r="AP11" s="25">
         <v>317863</v>
       </c>
-      <c r="AM11" s="21">
+      <c r="AQ11" s="21">
         <v>1103351</v>
       </c>
     </row>
-    <row r="16" spans="2:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="2:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="65" t="s">
+      <c r="E17" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="66"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="66"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="66"/>
-      <c r="L17" s="66"/>
-      <c r="M17" s="66"/>
-      <c r="N17" s="66"/>
-      <c r="O17" s="66"/>
-      <c r="P17" s="66"/>
-      <c r="Q17" s="66"/>
-      <c r="R17" s="66"/>
-      <c r="S17" s="66"/>
-      <c r="T17" s="66"/>
-      <c r="U17" s="66"/>
-      <c r="V17" s="66"/>
-      <c r="W17" s="66"/>
-      <c r="X17" s="66"/>
-      <c r="Y17" s="66"/>
-      <c r="Z17" s="66"/>
-      <c r="AA17" s="66"/>
-      <c r="AB17" s="66"/>
-      <c r="AC17" s="66"/>
-      <c r="AD17" s="66"/>
-      <c r="AE17" s="66"/>
-      <c r="AF17" s="66"/>
-      <c r="AG17" s="66"/>
-      <c r="AH17" s="66"/>
-      <c r="AI17" s="67"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="41"/>
+      <c r="R17" s="41"/>
+      <c r="S17" s="41"/>
+      <c r="T17" s="41"/>
+      <c r="U17" s="41"/>
+      <c r="V17" s="41"/>
+      <c r="W17" s="41"/>
+      <c r="X17" s="41"/>
+      <c r="Y17" s="41"/>
+      <c r="Z17" s="41"/>
+      <c r="AA17" s="41"/>
+      <c r="AB17" s="41"/>
+      <c r="AC17" s="41"/>
+      <c r="AD17" s="41"/>
+      <c r="AE17" s="41"/>
+      <c r="AF17" s="41"/>
+      <c r="AG17" s="41"/>
+      <c r="AH17" s="41"/>
+      <c r="AI17" s="42"/>
     </row>
     <row r="18" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="30"/>
+      <c r="D18" s="61"/>
       <c r="E18" s="2">
         <v>1</v>
       </c>
@@ -1991,60 +2206,60 @@
       <c r="T18" s="14">
         <v>16</v>
       </c>
-      <c r="U18" s="63">
+      <c r="U18" s="14">
         <v>17</v>
       </c>
-      <c r="V18" s="63">
+      <c r="V18" s="14">
         <v>20</v>
       </c>
-      <c r="W18" s="63">
+      <c r="W18" s="14">
         <v>30</v>
       </c>
-      <c r="X18" s="63">
+      <c r="X18" s="14">
         <v>40</v>
       </c>
-      <c r="Y18" s="63">
+      <c r="Y18" s="14">
         <v>50</v>
       </c>
-      <c r="Z18" s="63">
+      <c r="Z18" s="14">
         <v>60</v>
       </c>
-      <c r="AA18" s="63">
+      <c r="AA18" s="14">
         <v>70</v>
       </c>
-      <c r="AB18" s="63">
+      <c r="AB18" s="14">
         <v>80</v>
       </c>
-      <c r="AC18" s="63">
+      <c r="AC18" s="14">
         <v>100</v>
       </c>
-      <c r="AD18" s="63">
+      <c r="AD18" s="14">
         <v>120</v>
       </c>
-      <c r="AE18" s="63">
+      <c r="AE18" s="14">
         <v>140</v>
       </c>
-      <c r="AF18" s="63">
+      <c r="AF18" s="14">
         <v>200</v>
       </c>
-      <c r="AG18" s="63">
+      <c r="AG18" s="14">
         <v>1000</v>
       </c>
-      <c r="AH18" s="63">
+      <c r="AH18" s="14">
         <v>10000</v>
       </c>
-      <c r="AI18" s="64">
+      <c r="AI18" s="3">
         <v>15000</v>
       </c>
     </row>
     <row r="19" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="35"/>
+      <c r="D19" s="62"/>
       <c r="E19" s="11">
         <v>41421</v>
       </c>
@@ -2093,58 +2308,58 @@
       <c r="T19" s="28">
         <v>7675</v>
       </c>
-      <c r="U19" s="61">
+      <c r="U19" s="28">
         <v>7560</v>
       </c>
-      <c r="V19" s="61">
+      <c r="V19" s="28">
         <v>7576</v>
       </c>
-      <c r="W19" s="61">
+      <c r="W19" s="28">
         <v>9052</v>
       </c>
-      <c r="X19" s="61">
+      <c r="X19" s="28">
         <v>7539</v>
       </c>
-      <c r="Y19" s="61">
+      <c r="Y19" s="28">
         <v>7621</v>
       </c>
-      <c r="Z19" s="61">
+      <c r="Z19" s="28">
         <v>7574</v>
       </c>
-      <c r="AA19" s="61">
+      <c r="AA19" s="28">
         <v>7573</v>
       </c>
-      <c r="AB19" s="61">
+      <c r="AB19" s="28">
         <v>7560</v>
       </c>
-      <c r="AC19" s="61">
+      <c r="AC19" s="28">
         <v>7571</v>
       </c>
-      <c r="AD19" s="61">
+      <c r="AD19" s="28">
         <v>7578</v>
       </c>
-      <c r="AE19" s="61">
+      <c r="AE19" s="28">
         <v>7554</v>
       </c>
-      <c r="AF19" s="61">
+      <c r="AF19" s="28">
         <v>7591</v>
       </c>
-      <c r="AG19" s="61">
+      <c r="AG19" s="28">
         <v>7592</v>
       </c>
-      <c r="AH19" s="61">
+      <c r="AH19" s="28">
         <v>7787</v>
       </c>
-      <c r="AI19" s="62">
+      <c r="AI19" s="33">
         <v>7957</v>
       </c>
     </row>
     <row r="20" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="32"/>
-      <c r="C20" s="36" t="s">
+      <c r="B20" s="46"/>
+      <c r="C20" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="37"/>
+      <c r="D20" s="63"/>
       <c r="E20" s="4">
         <v>26094</v>
       </c>
@@ -2193,58 +2408,58 @@
       <c r="T20" s="26">
         <v>4317</v>
       </c>
-      <c r="U20" s="57">
+      <c r="U20" s="26">
         <v>4175</v>
       </c>
-      <c r="V20" s="57">
+      <c r="V20" s="26">
         <v>4196</v>
       </c>
-      <c r="W20" s="57">
+      <c r="W20" s="26">
         <v>4930</v>
       </c>
-      <c r="X20" s="57">
+      <c r="X20" s="26">
         <v>4189</v>
       </c>
-      <c r="Y20" s="57">
+      <c r="Y20" s="26">
         <v>4206</v>
       </c>
-      <c r="Z20" s="57">
+      <c r="Z20" s="26">
         <v>4228</v>
       </c>
-      <c r="AA20" s="57">
+      <c r="AA20" s="26">
         <v>4173</v>
       </c>
-      <c r="AB20" s="57">
+      <c r="AB20" s="26">
         <v>4184</v>
       </c>
-      <c r="AC20" s="57">
+      <c r="AC20" s="26">
         <v>4176</v>
       </c>
-      <c r="AD20" s="57">
+      <c r="AD20" s="26">
         <v>4179</v>
       </c>
-      <c r="AE20" s="57">
+      <c r="AE20" s="26">
         <v>4190</v>
       </c>
-      <c r="AF20" s="57">
+      <c r="AF20" s="26">
         <v>4205</v>
       </c>
-      <c r="AG20" s="57">
+      <c r="AG20" s="26">
         <v>4171</v>
       </c>
-      <c r="AH20" s="57">
+      <c r="AH20" s="26">
         <v>4403</v>
       </c>
-      <c r="AI20" s="58">
+      <c r="AI20" s="31">
         <v>4480</v>
       </c>
     </row>
     <row r="21" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="32"/>
-      <c r="C21" s="34" t="s">
+      <c r="B21" s="46"/>
+      <c r="C21" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="35"/>
+      <c r="D21" s="62"/>
       <c r="E21" s="4">
         <v>15331</v>
       </c>
@@ -2293,58 +2508,58 @@
       <c r="T21" s="26">
         <v>2495</v>
       </c>
-      <c r="U21" s="57">
+      <c r="U21" s="26">
         <v>2402</v>
       </c>
-      <c r="V21" s="57">
+      <c r="V21" s="26">
         <v>2405</v>
       </c>
-      <c r="W21" s="57">
+      <c r="W21" s="26">
         <v>2924</v>
       </c>
-      <c r="X21" s="57">
+      <c r="X21" s="26">
         <v>2416</v>
       </c>
-      <c r="Y21" s="57">
+      <c r="Y21" s="26">
         <v>2422</v>
       </c>
-      <c r="Z21" s="57">
+      <c r="Z21" s="26">
         <v>2581</v>
       </c>
-      <c r="AA21" s="57">
+      <c r="AA21" s="26">
         <v>2401</v>
       </c>
-      <c r="AB21" s="57">
+      <c r="AB21" s="26">
         <v>2403</v>
       </c>
-      <c r="AC21" s="57">
+      <c r="AC21" s="26">
         <v>2404</v>
       </c>
-      <c r="AD21" s="57">
+      <c r="AD21" s="26">
         <v>2399</v>
       </c>
-      <c r="AE21" s="57">
+      <c r="AE21" s="26">
         <v>2401</v>
       </c>
-      <c r="AF21" s="57">
+      <c r="AF21" s="26">
         <v>2415</v>
       </c>
-      <c r="AG21" s="57">
+      <c r="AG21" s="26">
         <v>2414</v>
       </c>
-      <c r="AH21" s="57">
+      <c r="AH21" s="26">
         <v>2618</v>
       </c>
-      <c r="AI21" s="58">
+      <c r="AI21" s="31">
         <v>2734</v>
       </c>
     </row>
     <row r="22" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="33"/>
-      <c r="C22" s="38" t="s">
+      <c r="B22" s="47"/>
+      <c r="C22" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="39"/>
+      <c r="D22" s="64"/>
       <c r="E22" s="6">
         <v>1107273</v>
       </c>
@@ -2393,57 +2608,900 @@
       <c r="T22" s="27">
         <v>209233</v>
       </c>
-      <c r="U22" s="59">
+      <c r="U22" s="27">
         <v>205155</v>
       </c>
-      <c r="V22" s="59">
+      <c r="V22" s="27">
         <v>200775</v>
       </c>
-      <c r="W22" s="59">
+      <c r="W22" s="27">
         <v>213393</v>
       </c>
-      <c r="X22" s="59">
+      <c r="X22" s="27">
         <v>186159</v>
       </c>
-      <c r="Y22" s="59">
+      <c r="Y22" s="27">
         <v>199143</v>
       </c>
-      <c r="Z22" s="59">
+      <c r="Z22" s="27">
         <v>209858</v>
       </c>
-      <c r="AA22" s="59">
+      <c r="AA22" s="27">
         <v>207626</v>
       </c>
-      <c r="AB22" s="59">
+      <c r="AB22" s="27">
         <v>206395</v>
       </c>
-      <c r="AC22" s="59">
+      <c r="AC22" s="27">
         <v>207235</v>
       </c>
-      <c r="AD22" s="59">
+      <c r="AD22" s="27">
         <v>207126</v>
       </c>
-      <c r="AE22" s="59">
+      <c r="AE22" s="27">
         <v>206120</v>
       </c>
-      <c r="AF22" s="59">
+      <c r="AF22" s="27">
         <v>206035</v>
       </c>
-      <c r="AG22" s="59">
+      <c r="AG22" s="27">
         <v>205114</v>
       </c>
-      <c r="AH22" s="59">
+      <c r="AH22" s="27">
         <v>200946</v>
       </c>
-      <c r="AI22" s="60">
+      <c r="AI22" s="32">
         <v>204284</v>
+      </c>
+    </row>
+    <row r="35" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E36" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="41"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="41"/>
+      <c r="L36" s="41"/>
+      <c r="M36" s="41"/>
+      <c r="N36" s="41"/>
+      <c r="O36" s="41"/>
+      <c r="P36" s="41"/>
+      <c r="Q36" s="41"/>
+      <c r="R36" s="41"/>
+      <c r="S36" s="41"/>
+      <c r="T36" s="41"/>
+      <c r="U36" s="41"/>
+      <c r="V36" s="41"/>
+      <c r="W36" s="41"/>
+      <c r="X36" s="41"/>
+      <c r="Y36" s="41"/>
+      <c r="Z36" s="41"/>
+      <c r="AA36" s="41"/>
+      <c r="AB36" s="41"/>
+      <c r="AC36" s="41"/>
+      <c r="AD36" s="41"/>
+      <c r="AE36" s="41"/>
+      <c r="AF36" s="41"/>
+      <c r="AG36" s="41"/>
+      <c r="AH36" s="41"/>
+      <c r="AI36" s="41"/>
+      <c r="AJ36" s="41"/>
+      <c r="AK36" s="41"/>
+      <c r="AL36" s="41"/>
+      <c r="AM36" s="41"/>
+      <c r="AN36" s="41"/>
+      <c r="AO36" s="41"/>
+      <c r="AP36" s="41"/>
+      <c r="AQ36" s="41"/>
+      <c r="AR36" s="41"/>
+      <c r="AS36" s="41"/>
+      <c r="AT36" s="41"/>
+      <c r="AU36" s="41"/>
+      <c r="AV36" s="42"/>
+    </row>
+    <row r="37" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="61"/>
+      <c r="E37" s="68">
+        <v>1</v>
+      </c>
+      <c r="F37" s="66">
+        <v>2</v>
+      </c>
+      <c r="G37" s="66">
+        <v>3</v>
+      </c>
+      <c r="H37" s="66">
+        <v>4</v>
+      </c>
+      <c r="I37" s="66">
+        <v>5</v>
+      </c>
+      <c r="J37" s="66">
+        <v>6</v>
+      </c>
+      <c r="K37" s="66">
+        <v>7</v>
+      </c>
+      <c r="L37" s="66">
+        <v>8</v>
+      </c>
+      <c r="M37" s="66">
+        <v>9</v>
+      </c>
+      <c r="N37" s="66">
+        <v>10</v>
+      </c>
+      <c r="O37" s="66">
+        <v>11</v>
+      </c>
+      <c r="P37" s="66">
+        <v>12</v>
+      </c>
+      <c r="Q37" s="66">
+        <v>13</v>
+      </c>
+      <c r="R37" s="66">
+        <v>14</v>
+      </c>
+      <c r="S37" s="66">
+        <v>15</v>
+      </c>
+      <c r="T37" s="66">
+        <v>16</v>
+      </c>
+      <c r="U37" s="66">
+        <v>17</v>
+      </c>
+      <c r="V37" s="66">
+        <v>20</v>
+      </c>
+      <c r="W37" s="66">
+        <v>30</v>
+      </c>
+      <c r="X37" s="66">
+        <v>40</v>
+      </c>
+      <c r="Y37" s="66">
+        <v>50</v>
+      </c>
+      <c r="Z37" s="66">
+        <v>60</v>
+      </c>
+      <c r="AA37" s="66">
+        <v>70</v>
+      </c>
+      <c r="AB37" s="66">
+        <v>80</v>
+      </c>
+      <c r="AC37" s="66">
+        <v>90</v>
+      </c>
+      <c r="AD37" s="66">
+        <v>100</v>
+      </c>
+      <c r="AE37" s="66">
+        <v>120</v>
+      </c>
+      <c r="AF37" s="66">
+        <v>140</v>
+      </c>
+      <c r="AG37" s="66">
+        <v>175</v>
+      </c>
+      <c r="AH37" s="66">
+        <v>200</v>
+      </c>
+      <c r="AI37" s="67">
+        <v>225</v>
+      </c>
+      <c r="AJ37" s="81">
+        <v>250</v>
+      </c>
+      <c r="AK37" s="67">
+        <v>275</v>
+      </c>
+      <c r="AL37" s="73">
+        <v>280</v>
+      </c>
+      <c r="AM37" s="76">
+        <v>285</v>
+      </c>
+      <c r="AN37" s="76">
+        <v>290</v>
+      </c>
+      <c r="AO37" s="76">
+        <v>295</v>
+      </c>
+      <c r="AP37" s="66">
+        <v>300</v>
+      </c>
+      <c r="AQ37" s="67">
+        <v>325</v>
+      </c>
+      <c r="AR37" s="66">
+        <v>350</v>
+      </c>
+      <c r="AS37" s="67">
+        <v>375</v>
+      </c>
+      <c r="AT37" s="66">
+        <v>400</v>
+      </c>
+      <c r="AU37" s="67">
+        <v>425</v>
+      </c>
+      <c r="AV37" s="18">
+        <v>450</v>
+      </c>
+      <c r="AW37" s="73"/>
+      <c r="AX37" s="73"/>
+      <c r="AY37" s="73"/>
+      <c r="AZ37" s="73"/>
+      <c r="BA37" s="73"/>
+      <c r="BB37" s="73"/>
+    </row>
+    <row r="38" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="62"/>
+      <c r="E38" s="69">
+        <v>41768</v>
+      </c>
+      <c r="F38" s="70">
+        <v>20910</v>
+      </c>
+      <c r="G38" s="70">
+        <v>13985</v>
+      </c>
+      <c r="H38" s="70">
+        <v>10483</v>
+      </c>
+      <c r="I38" s="70">
+        <v>8404</v>
+      </c>
+      <c r="J38" s="70">
+        <v>7023</v>
+      </c>
+      <c r="K38" s="70">
+        <v>6030</v>
+      </c>
+      <c r="L38" s="70">
+        <v>5270</v>
+      </c>
+      <c r="M38" s="70">
+        <v>4698</v>
+      </c>
+      <c r="N38" s="70">
+        <v>4223</v>
+      </c>
+      <c r="O38" s="70">
+        <v>3862</v>
+      </c>
+      <c r="P38" s="70">
+        <v>3542</v>
+      </c>
+      <c r="Q38" s="70">
+        <v>3270</v>
+      </c>
+      <c r="R38" s="70">
+        <v>3059</v>
+      </c>
+      <c r="S38" s="70">
+        <v>2831</v>
+      </c>
+      <c r="T38" s="70">
+        <v>2597</v>
+      </c>
+      <c r="U38" s="70">
+        <v>2538</v>
+      </c>
+      <c r="V38" s="70">
+        <v>2134</v>
+      </c>
+      <c r="W38" s="70">
+        <v>1436</v>
+      </c>
+      <c r="X38" s="70">
+        <v>1085</v>
+      </c>
+      <c r="Y38" s="70">
+        <v>930</v>
+      </c>
+      <c r="Z38" s="70">
+        <v>794</v>
+      </c>
+      <c r="AA38" s="70">
+        <v>753</v>
+      </c>
+      <c r="AB38" s="70">
+        <v>659</v>
+      </c>
+      <c r="AC38" s="70">
+        <v>611</v>
+      </c>
+      <c r="AD38" s="70">
+        <v>574</v>
+      </c>
+      <c r="AE38" s="70">
+        <v>524</v>
+      </c>
+      <c r="AF38" s="70">
+        <v>482</v>
+      </c>
+      <c r="AG38" s="70">
+        <v>428</v>
+      </c>
+      <c r="AH38" s="70">
+        <v>410</v>
+      </c>
+      <c r="AI38" s="70">
+        <v>387</v>
+      </c>
+      <c r="AJ38" s="82">
+        <v>391</v>
+      </c>
+      <c r="AK38" s="71">
+        <v>392</v>
+      </c>
+      <c r="AL38" s="76">
+        <v>406</v>
+      </c>
+      <c r="AM38" s="71">
+        <v>402</v>
+      </c>
+      <c r="AN38" s="71">
+        <v>403</v>
+      </c>
+      <c r="AO38" s="71">
+        <v>404</v>
+      </c>
+      <c r="AP38" s="71">
+        <v>404</v>
+      </c>
+      <c r="AQ38" s="71">
+        <v>402</v>
+      </c>
+      <c r="AR38" s="71">
+        <v>405</v>
+      </c>
+      <c r="AS38" s="71">
+        <v>408</v>
+      </c>
+      <c r="AT38" s="71">
+        <v>407</v>
+      </c>
+      <c r="AU38" s="71">
+        <v>410</v>
+      </c>
+      <c r="AV38" s="72">
+        <v>410</v>
+      </c>
+      <c r="AW38" s="74"/>
+      <c r="AX38" s="75"/>
+      <c r="AY38" s="75"/>
+      <c r="AZ38" s="75"/>
+      <c r="BA38" s="75"/>
+      <c r="BB38" s="75"/>
+    </row>
+    <row r="39" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="46"/>
+      <c r="C39" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="63"/>
+      <c r="E39" s="4">
+        <v>23012</v>
+      </c>
+      <c r="F39" s="1">
+        <v>11529</v>
+      </c>
+      <c r="G39" s="1">
+        <v>7748</v>
+      </c>
+      <c r="H39" s="1">
+        <v>5829</v>
+      </c>
+      <c r="I39" s="1">
+        <v>4652</v>
+      </c>
+      <c r="J39" s="1">
+        <v>3885</v>
+      </c>
+      <c r="K39" s="1">
+        <v>3339</v>
+      </c>
+      <c r="L39" s="1">
+        <v>2925</v>
+      </c>
+      <c r="M39" s="1">
+        <v>2606</v>
+      </c>
+      <c r="N39" s="1">
+        <v>2347</v>
+      </c>
+      <c r="O39" s="1">
+        <v>2140</v>
+      </c>
+      <c r="P39" s="1">
+        <v>1693</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>1811</v>
+      </c>
+      <c r="R39" s="1">
+        <v>1690</v>
+      </c>
+      <c r="S39" s="1">
+        <v>1581</v>
+      </c>
+      <c r="T39" s="1">
+        <v>1484</v>
+      </c>
+      <c r="U39" s="1">
+        <v>1398</v>
+      </c>
+      <c r="V39" s="1">
+        <v>1193</v>
+      </c>
+      <c r="W39" s="1">
+        <v>832</v>
+      </c>
+      <c r="X39" s="1">
+        <v>614</v>
+      </c>
+      <c r="Y39" s="1">
+        <v>517</v>
+      </c>
+      <c r="Z39" s="1">
+        <v>455</v>
+      </c>
+      <c r="AA39" s="1">
+        <v>409</v>
+      </c>
+      <c r="AB39" s="1">
+        <v>384</v>
+      </c>
+      <c r="AC39" s="1">
+        <v>355</v>
+      </c>
+      <c r="AD39" s="1">
+        <v>331</v>
+      </c>
+      <c r="AE39" s="1">
+        <v>309</v>
+      </c>
+      <c r="AF39" s="1">
+        <v>287</v>
+      </c>
+      <c r="AG39" s="1">
+        <v>263</v>
+      </c>
+      <c r="AH39" s="1">
+        <v>251</v>
+      </c>
+      <c r="AI39" s="1">
+        <v>244</v>
+      </c>
+      <c r="AJ39" s="83">
+        <v>245</v>
+      </c>
+      <c r="AK39" s="26">
+        <v>247</v>
+      </c>
+      <c r="AL39" s="26">
+        <v>253</v>
+      </c>
+      <c r="AM39" s="26">
+        <v>252</v>
+      </c>
+      <c r="AN39" s="26">
+        <v>253</v>
+      </c>
+      <c r="AO39" s="26">
+        <v>252</v>
+      </c>
+      <c r="AP39" s="26">
+        <v>254</v>
+      </c>
+      <c r="AQ39" s="26">
+        <v>251</v>
+      </c>
+      <c r="AR39" s="26">
+        <v>252</v>
+      </c>
+      <c r="AS39" s="26">
+        <v>254</v>
+      </c>
+      <c r="AT39" s="26">
+        <v>253</v>
+      </c>
+      <c r="AU39" s="26">
+        <v>255</v>
+      </c>
+      <c r="AV39" s="31">
+        <v>265</v>
+      </c>
+      <c r="AW39" s="74"/>
+      <c r="AX39" s="75"/>
+      <c r="AY39" s="75"/>
+      <c r="AZ39" s="75"/>
+      <c r="BA39" s="75"/>
+      <c r="BB39" s="75"/>
+    </row>
+    <row r="40" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="46"/>
+      <c r="C40" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="62"/>
+      <c r="E40" s="4">
+        <v>13545</v>
+      </c>
+      <c r="F40" s="1">
+        <v>6783</v>
+      </c>
+      <c r="G40" s="1">
+        <v>4558</v>
+      </c>
+      <c r="H40" s="1">
+        <v>3421</v>
+      </c>
+      <c r="I40" s="1">
+        <v>2744</v>
+      </c>
+      <c r="J40" s="1">
+        <v>2301</v>
+      </c>
+      <c r="K40" s="1">
+        <v>1999</v>
+      </c>
+      <c r="L40" s="1">
+        <v>1741</v>
+      </c>
+      <c r="M40" s="1">
+        <v>1552</v>
+      </c>
+      <c r="N40" s="1">
+        <v>1398</v>
+      </c>
+      <c r="O40" s="1">
+        <v>1272</v>
+      </c>
+      <c r="P40" s="1">
+        <v>1169</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>1082</v>
+      </c>
+      <c r="R40" s="1">
+        <v>1003</v>
+      </c>
+      <c r="S40" s="1">
+        <v>938</v>
+      </c>
+      <c r="T40" s="1">
+        <v>879</v>
+      </c>
+      <c r="U40" s="1">
+        <v>832</v>
+      </c>
+      <c r="V40" s="1">
+        <v>718</v>
+      </c>
+      <c r="W40" s="1">
+        <v>486</v>
+      </c>
+      <c r="X40" s="1">
+        <v>391</v>
+      </c>
+      <c r="Y40" s="1">
+        <v>314</v>
+      </c>
+      <c r="Z40" s="1">
+        <v>279</v>
+      </c>
+      <c r="AA40" s="1">
+        <v>253</v>
+      </c>
+      <c r="AB40" s="1">
+        <v>235</v>
+      </c>
+      <c r="AC40" s="1">
+        <v>222</v>
+      </c>
+      <c r="AD40" s="1">
+        <v>209</v>
+      </c>
+      <c r="AE40" s="1">
+        <v>197</v>
+      </c>
+      <c r="AF40" s="1">
+        <v>188</v>
+      </c>
+      <c r="AG40" s="1">
+        <v>176</v>
+      </c>
+      <c r="AH40" s="1">
+        <v>170</v>
+      </c>
+      <c r="AI40" s="1">
+        <v>166</v>
+      </c>
+      <c r="AJ40" s="83">
+        <v>165</v>
+      </c>
+      <c r="AK40" s="26">
+        <v>167</v>
+      </c>
+      <c r="AL40" s="26">
+        <v>169</v>
+      </c>
+      <c r="AM40" s="26">
+        <v>169</v>
+      </c>
+      <c r="AN40" s="26">
+        <v>171</v>
+      </c>
+      <c r="AO40" s="26">
+        <v>169</v>
+      </c>
+      <c r="AP40" s="26">
+        <v>170</v>
+      </c>
+      <c r="AQ40" s="26">
+        <v>178</v>
+      </c>
+      <c r="AR40" s="26">
+        <v>170</v>
+      </c>
+      <c r="AS40" s="26">
+        <v>171</v>
+      </c>
+      <c r="AT40" s="26">
+        <v>170</v>
+      </c>
+      <c r="AU40" s="26">
+        <v>178</v>
+      </c>
+      <c r="AV40" s="31">
+        <v>171</v>
+      </c>
+      <c r="AW40" s="74"/>
+      <c r="AX40" s="75"/>
+      <c r="AY40" s="75"/>
+      <c r="AZ40" s="75"/>
+      <c r="BA40" s="75"/>
+      <c r="BB40" s="75"/>
+    </row>
+    <row r="41" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="47"/>
+      <c r="C41" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="64"/>
+      <c r="E41" s="6">
+        <v>1076471</v>
+      </c>
+      <c r="F41" s="7">
+        <v>535391</v>
+      </c>
+      <c r="G41" s="7">
+        <v>357585</v>
+      </c>
+      <c r="H41" s="7">
+        <v>267984</v>
+      </c>
+      <c r="I41" s="7">
+        <v>214341</v>
+      </c>
+      <c r="J41" s="7">
+        <v>178581</v>
+      </c>
+      <c r="K41" s="7">
+        <v>153075</v>
+      </c>
+      <c r="L41" s="7">
+        <v>133907</v>
+      </c>
+      <c r="M41" s="7">
+        <v>119102</v>
+      </c>
+      <c r="N41" s="7">
+        <v>107170</v>
+      </c>
+      <c r="O41" s="7">
+        <v>97426</v>
+      </c>
+      <c r="P41" s="7">
+        <v>89300</v>
+      </c>
+      <c r="Q41" s="7">
+        <v>82454</v>
+      </c>
+      <c r="R41" s="7">
+        <v>76563</v>
+      </c>
+      <c r="S41" s="7">
+        <v>71476</v>
+      </c>
+      <c r="T41" s="7">
+        <v>67018</v>
+      </c>
+      <c r="U41" s="7">
+        <v>63126</v>
+      </c>
+      <c r="V41" s="7">
+        <v>53687</v>
+      </c>
+      <c r="W41" s="7">
+        <v>35828</v>
+      </c>
+      <c r="X41" s="7">
+        <v>26996</v>
+      </c>
+      <c r="Y41" s="7">
+        <v>22060</v>
+      </c>
+      <c r="Z41" s="7">
+        <v>19853</v>
+      </c>
+      <c r="AA41" s="7">
+        <v>17745</v>
+      </c>
+      <c r="AB41" s="7">
+        <v>16436</v>
+      </c>
+      <c r="AC41" s="7">
+        <v>15197</v>
+      </c>
+      <c r="AD41" s="7">
+        <v>14025</v>
+      </c>
+      <c r="AE41" s="7">
+        <v>12200</v>
+      </c>
+      <c r="AF41" s="7">
+        <v>11237</v>
+      </c>
+      <c r="AG41" s="7">
+        <v>9952</v>
+      </c>
+      <c r="AH41" s="7">
+        <v>9373</v>
+      </c>
+      <c r="AI41" s="7">
+        <v>8955</v>
+      </c>
+      <c r="AJ41" s="84">
+        <v>8926</v>
+      </c>
+      <c r="AK41" s="27">
+        <v>8978</v>
+      </c>
+      <c r="AL41" s="27">
+        <v>9422</v>
+      </c>
+      <c r="AM41" s="27">
+        <v>9435</v>
+      </c>
+      <c r="AN41" s="27">
+        <v>9447</v>
+      </c>
+      <c r="AO41" s="27">
+        <v>9343</v>
+      </c>
+      <c r="AP41" s="27">
+        <v>9373</v>
+      </c>
+      <c r="AQ41" s="27">
+        <v>9396</v>
+      </c>
+      <c r="AR41" s="27">
+        <v>9453</v>
+      </c>
+      <c r="AS41" s="27">
+        <v>9493</v>
+      </c>
+      <c r="AT41" s="27">
+        <v>9447</v>
+      </c>
+      <c r="AU41" s="27">
+        <v>9533</v>
+      </c>
+      <c r="AV41" s="32">
+        <v>9533</v>
+      </c>
+      <c r="AW41" s="74"/>
+      <c r="AX41" s="75"/>
+      <c r="AY41" s="75"/>
+      <c r="AZ41" s="75"/>
+      <c r="BA41" s="75"/>
+      <c r="BB41" s="75"/>
+    </row>
+    <row r="43" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="65"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="65"/>
+    </row>
+    <row r="44" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="61"/>
+      <c r="E44" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="62"/>
+      <c r="E45" s="19">
+        <v>28218</v>
+      </c>
+    </row>
+    <row r="46" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="63"/>
+      <c r="E46" s="20">
+        <v>14757</v>
+      </c>
+    </row>
+    <row r="47" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="62"/>
+      <c r="E47" s="20">
+        <v>8108</v>
+      </c>
+    </row>
+    <row r="48" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C48" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="64"/>
+      <c r="E48" s="21">
+        <v>898369</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="E3:AL4"/>
+  <mergeCells count="32">
+    <mergeCell ref="E36:AV36"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E3:AP4"/>
     <mergeCell ref="E17:AI17"/>
-    <mergeCell ref="AM5:AM6"/>
+    <mergeCell ref="AQ5:AQ6"/>
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
@@ -2454,14 +3512,9 @@
     <mergeCell ref="E5:O6"/>
     <mergeCell ref="P5:Z6"/>
     <mergeCell ref="AA5:AK6"/>
-    <mergeCell ref="AL5:AL6"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="AP5:AP6"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final profiling and plots added
</commit_message>
<xml_diff>
--- a/Profiling OMP/DHPC.xlsx
+++ b/Profiling OMP/DHPC.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francisco Câmara\OneDrive\Ambiente de Trabalho\DHPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058C2457-A023-44D0-B287-5598C8DE9CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D897B9CF-AE05-4D5A-A1B3-D559B9A57869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Folha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="19">
   <si>
     <t>Scheduling Type</t>
   </si>
@@ -74,6 +75,15 @@
   <si>
     <t>Dynamic Chunk_size = 1</t>
   </si>
+  <si>
+    <t>nThreads = 4 6000*4000 2000 iterations - dgxh100</t>
+  </si>
+  <si>
+    <t>n_threads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6000*4000 - 2000 iterations - chunk_size = 6 </t>
+  </si>
 </sst>
 </file>
 
@@ -100,7 +110,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,8 +141,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="55">
+  <borders count="62">
     <border>
       <left/>
       <right/>
@@ -820,11 +854,96 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -913,100 +1032,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1024,11 +1053,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1050,6 +1078,231 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1332,8 +1585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:BB48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V14" workbookViewId="0">
-      <selection activeCell="AK37" sqref="AK37:AN41"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AS9" sqref="AS9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,141 +1596,139 @@
   <sheetData>
     <row r="2" spans="2:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:50" x14ac:dyDescent="0.25">
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="35"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
-      <c r="U3" s="35"/>
-      <c r="V3" s="35"/>
-      <c r="W3" s="35"/>
-      <c r="X3" s="35"/>
-      <c r="Y3" s="35"/>
-      <c r="Z3" s="35"/>
-      <c r="AA3" s="35"/>
-      <c r="AB3" s="35"/>
-      <c r="AC3" s="35"/>
-      <c r="AD3" s="35"/>
-      <c r="AE3" s="35"/>
-      <c r="AF3" s="35"/>
-      <c r="AG3" s="35"/>
-      <c r="AH3" s="35"/>
-      <c r="AI3" s="35"/>
-      <c r="AJ3" s="35"/>
-      <c r="AK3" s="35"/>
-      <c r="AL3" s="35"/>
-      <c r="AM3" s="35"/>
-      <c r="AN3" s="35"/>
-      <c r="AO3" s="35"/>
-      <c r="AP3" s="36"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="59"/>
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="59"/>
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="59"/>
+      <c r="AC3" s="59"/>
+      <c r="AD3" s="59"/>
+      <c r="AE3" s="59"/>
+      <c r="AF3" s="59"/>
+      <c r="AG3" s="59"/>
+      <c r="AH3" s="59"/>
+      <c r="AI3" s="59"/>
+      <c r="AJ3" s="59"/>
+      <c r="AK3" s="59"/>
+      <c r="AL3" s="59"/>
+      <c r="AM3" s="59"/>
+      <c r="AN3" s="59"/>
+      <c r="AO3" s="59"/>
+      <c r="AP3" s="60"/>
     </row>
     <row r="4" spans="2:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="37"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
-      <c r="U4" s="38"/>
-      <c r="V4" s="38"/>
-      <c r="W4" s="38"/>
-      <c r="X4" s="38"/>
-      <c r="Y4" s="38"/>
-      <c r="Z4" s="38"/>
-      <c r="AA4" s="38"/>
-      <c r="AB4" s="38"/>
-      <c r="AC4" s="38"/>
-      <c r="AD4" s="38"/>
-      <c r="AE4" s="38"/>
-      <c r="AF4" s="38"/>
-      <c r="AG4" s="38"/>
-      <c r="AH4" s="38"/>
-      <c r="AI4" s="38"/>
-      <c r="AJ4" s="38"/>
-      <c r="AK4" s="38"/>
-      <c r="AL4" s="38"/>
-      <c r="AM4" s="38"/>
-      <c r="AN4" s="38"/>
-      <c r="AO4" s="38"/>
-      <c r="AP4" s="39"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="62"/>
+      <c r="P4" s="62"/>
+      <c r="Q4" s="62"/>
+      <c r="R4" s="62"/>
+      <c r="S4" s="62"/>
+      <c r="T4" s="62"/>
+      <c r="U4" s="62"/>
+      <c r="V4" s="62"/>
+      <c r="W4" s="62"/>
+      <c r="X4" s="62"/>
+      <c r="Y4" s="62"/>
+      <c r="Z4" s="62"/>
+      <c r="AA4" s="62"/>
+      <c r="AB4" s="62"/>
+      <c r="AC4" s="62"/>
+      <c r="AD4" s="62"/>
+      <c r="AE4" s="62"/>
+      <c r="AF4" s="62"/>
+      <c r="AG4" s="62"/>
+      <c r="AH4" s="62"/>
+      <c r="AI4" s="62"/>
+      <c r="AJ4" s="62"/>
+      <c r="AK4" s="62"/>
+      <c r="AL4" s="62"/>
+      <c r="AM4" s="62"/>
+      <c r="AN4" s="62"/>
+      <c r="AO4" s="62"/>
+      <c r="AP4" s="63"/>
     </row>
     <row r="5" spans="2:50" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="53"/>
-      <c r="E5" s="34" t="s">
+      <c r="D5" s="77"/>
+      <c r="E5" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="34" t="s">
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
-      <c r="T5" s="35"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="35"/>
-      <c r="W5" s="35"/>
-      <c r="X5" s="35"/>
-      <c r="Y5" s="35"/>
-      <c r="Z5" s="36"/>
-      <c r="AA5" s="34" t="s">
+      <c r="Q5" s="59"/>
+      <c r="R5" s="59"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="59"/>
+      <c r="V5" s="59"/>
+      <c r="W5" s="59"/>
+      <c r="X5" s="59"/>
+      <c r="Y5" s="59"/>
+      <c r="Z5" s="60"/>
+      <c r="AA5" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="AB5" s="35"/>
-      <c r="AC5" s="35"/>
-      <c r="AD5" s="35"/>
-      <c r="AE5" s="35"/>
-      <c r="AF5" s="35"/>
-      <c r="AG5" s="35"/>
-      <c r="AH5" s="35"/>
-      <c r="AI5" s="35"/>
-      <c r="AJ5" s="35"/>
-      <c r="AK5" s="36"/>
-      <c r="AL5" s="29"/>
-      <c r="AM5" s="29"/>
+      <c r="AB5" s="59"/>
+      <c r="AC5" s="59"/>
+      <c r="AD5" s="59"/>
+      <c r="AE5" s="59"/>
+      <c r="AF5" s="59"/>
+      <c r="AG5" s="59"/>
+      <c r="AH5" s="59"/>
+      <c r="AI5" s="59"/>
+      <c r="AJ5" s="59"/>
+      <c r="AK5" s="60"/>
+      <c r="AL5" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM5" s="67" t="s">
+        <v>13</v>
+      </c>
       <c r="AN5" s="29"/>
       <c r="AO5" s="29"/>
-      <c r="AP5" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="AQ5" s="43" t="s">
-        <v>13</v>
-      </c>
       <c r="AR5" s="15"/>
       <c r="AS5" s="15"/>
       <c r="AT5" s="15"/>
@@ -1487,47 +1738,45 @@
       <c r="AX5" s="15"/>
     </row>
     <row r="6" spans="2:50" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="54"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="38"/>
-      <c r="R6" s="38"/>
-      <c r="S6" s="38"/>
-      <c r="T6" s="38"/>
-      <c r="U6" s="38"/>
-      <c r="V6" s="38"/>
-      <c r="W6" s="38"/>
-      <c r="X6" s="38"/>
-      <c r="Y6" s="38"/>
-      <c r="Z6" s="39"/>
-      <c r="AA6" s="37"/>
-      <c r="AB6" s="38"/>
-      <c r="AC6" s="38"/>
-      <c r="AD6" s="38"/>
-      <c r="AE6" s="38"/>
-      <c r="AF6" s="38"/>
-      <c r="AG6" s="38"/>
-      <c r="AH6" s="38"/>
-      <c r="AI6" s="38"/>
-      <c r="AJ6" s="38"/>
-      <c r="AK6" s="39"/>
-      <c r="AL6" s="30"/>
-      <c r="AM6" s="30"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62"/>
+      <c r="N6" s="62"/>
+      <c r="O6" s="63"/>
+      <c r="P6" s="61"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="62"/>
+      <c r="S6" s="62"/>
+      <c r="T6" s="62"/>
+      <c r="U6" s="62"/>
+      <c r="V6" s="62"/>
+      <c r="W6" s="62"/>
+      <c r="X6" s="62"/>
+      <c r="Y6" s="62"/>
+      <c r="Z6" s="63"/>
+      <c r="AA6" s="61"/>
+      <c r="AB6" s="62"/>
+      <c r="AC6" s="62"/>
+      <c r="AD6" s="62"/>
+      <c r="AE6" s="62"/>
+      <c r="AF6" s="62"/>
+      <c r="AG6" s="62"/>
+      <c r="AH6" s="62"/>
+      <c r="AI6" s="62"/>
+      <c r="AJ6" s="62"/>
+      <c r="AK6" s="63"/>
+      <c r="AL6" s="84"/>
+      <c r="AM6" s="68"/>
       <c r="AN6" s="30"/>
       <c r="AO6" s="30"/>
-      <c r="AP6" s="60"/>
-      <c r="AQ6" s="44"/>
       <c r="AR6" s="15"/>
       <c r="AS6" s="15"/>
       <c r="AT6" s="15"/>
@@ -1537,10 +1786,10 @@
       <c r="AX6" s="15"/>
     </row>
     <row r="7" spans="2:50" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="57"/>
+      <c r="D7" s="81"/>
       <c r="E7" s="2">
         <v>1</v>
       </c>
@@ -1640,25 +1889,23 @@
       <c r="AK7" s="3">
         <v>1000</v>
       </c>
-      <c r="AL7" s="77"/>
-      <c r="AM7" s="77"/>
-      <c r="AN7" s="77"/>
-      <c r="AO7" s="77"/>
-      <c r="AP7" s="22" t="s">
+      <c r="AL7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="AQ7" s="18" t="s">
+      <c r="AM7" s="18" t="s">
         <v>12</v>
       </c>
+      <c r="AN7" s="46"/>
+      <c r="AO7" s="46"/>
     </row>
     <row r="8" spans="2:50" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="49"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="11">
         <v>7398</v>
       </c>
@@ -1758,23 +2005,21 @@
       <c r="AK8" s="13">
         <v>12719</v>
       </c>
-      <c r="AL8" s="78"/>
-      <c r="AM8" s="78"/>
-      <c r="AN8" s="78"/>
-      <c r="AO8" s="78"/>
-      <c r="AP8" s="23">
+      <c r="AL8" s="23">
         <v>14986</v>
       </c>
-      <c r="AQ8" s="19">
+      <c r="AM8" s="19">
         <v>48421</v>
       </c>
+      <c r="AN8" s="47"/>
+      <c r="AO8" s="47"/>
     </row>
     <row r="9" spans="2:50" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="46"/>
-      <c r="C9" s="58" t="s">
+      <c r="B9" s="70"/>
+      <c r="C9" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="59"/>
+      <c r="D9" s="83"/>
       <c r="E9" s="4">
         <v>4144</v>
       </c>
@@ -1874,23 +2119,21 @@
       <c r="AK9" s="5">
         <v>7495</v>
       </c>
-      <c r="AL9" s="79"/>
-      <c r="AM9" s="79"/>
-      <c r="AN9" s="79"/>
-      <c r="AO9" s="79"/>
-      <c r="AP9" s="24">
+      <c r="AL9" s="24">
         <v>9367</v>
       </c>
-      <c r="AQ9" s="20">
+      <c r="AM9" s="20">
         <v>26219</v>
       </c>
+      <c r="AN9" s="48"/>
+      <c r="AO9" s="48"/>
     </row>
     <row r="10" spans="2:50" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="46"/>
-      <c r="C10" s="48" t="s">
+      <c r="B10" s="70"/>
+      <c r="C10" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="49"/>
+      <c r="D10" s="73"/>
       <c r="E10" s="4">
         <v>2385</v>
       </c>
@@ -1990,23 +2233,21 @@
       <c r="AK10" s="5">
         <v>6304</v>
       </c>
-      <c r="AL10" s="79"/>
-      <c r="AM10" s="79"/>
-      <c r="AN10" s="79"/>
-      <c r="AO10" s="79"/>
-      <c r="AP10" s="24">
+      <c r="AL10" s="24">
         <v>5364</v>
       </c>
-      <c r="AQ10" s="20">
+      <c r="AM10" s="20">
         <v>15398</v>
       </c>
+      <c r="AN10" s="48"/>
+      <c r="AO10" s="48"/>
     </row>
     <row r="11" spans="2:50" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="47"/>
-      <c r="C11" s="50" t="s">
+      <c r="B11" s="71"/>
+      <c r="C11" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="51"/>
+      <c r="D11" s="75"/>
       <c r="E11" s="6">
         <v>180093</v>
       </c>
@@ -2106,58 +2347,56 @@
       <c r="AK11" s="8">
         <v>274438</v>
       </c>
-      <c r="AL11" s="80"/>
-      <c r="AM11" s="80"/>
-      <c r="AN11" s="80"/>
-      <c r="AO11" s="80"/>
-      <c r="AP11" s="25">
+      <c r="AL11" s="25">
         <v>317863</v>
       </c>
-      <c r="AQ11" s="21">
+      <c r="AM11" s="21">
         <v>1103351</v>
       </c>
+      <c r="AN11" s="49"/>
+      <c r="AO11" s="49"/>
     </row>
     <row r="16" spans="2:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="40" t="s">
+      <c r="E17" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="41"/>
-      <c r="N17" s="41"/>
-      <c r="O17" s="41"/>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="41"/>
-      <c r="R17" s="41"/>
-      <c r="S17" s="41"/>
-      <c r="T17" s="41"/>
-      <c r="U17" s="41"/>
-      <c r="V17" s="41"/>
-      <c r="W17" s="41"/>
-      <c r="X17" s="41"/>
-      <c r="Y17" s="41"/>
-      <c r="Z17" s="41"/>
-      <c r="AA17" s="41"/>
-      <c r="AB17" s="41"/>
-      <c r="AC17" s="41"/>
-      <c r="AD17" s="41"/>
-      <c r="AE17" s="41"/>
-      <c r="AF17" s="41"/>
-      <c r="AG17" s="41"/>
-      <c r="AH17" s="41"/>
-      <c r="AI17" s="42"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
+      <c r="M17" s="65"/>
+      <c r="N17" s="65"/>
+      <c r="O17" s="65"/>
+      <c r="P17" s="65"/>
+      <c r="Q17" s="65"/>
+      <c r="R17" s="65"/>
+      <c r="S17" s="65"/>
+      <c r="T17" s="65"/>
+      <c r="U17" s="65"/>
+      <c r="V17" s="65"/>
+      <c r="W17" s="65"/>
+      <c r="X17" s="65"/>
+      <c r="Y17" s="65"/>
+      <c r="Z17" s="65"/>
+      <c r="AA17" s="65"/>
+      <c r="AB17" s="65"/>
+      <c r="AC17" s="65"/>
+      <c r="AD17" s="65"/>
+      <c r="AE17" s="65"/>
+      <c r="AF17" s="65"/>
+      <c r="AG17" s="65"/>
+      <c r="AH17" s="65"/>
+      <c r="AI17" s="66"/>
     </row>
     <row r="18" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="61"/>
+      <c r="D18" s="85"/>
       <c r="E18" s="2">
         <v>1</v>
       </c>
@@ -2253,13 +2492,13 @@
       </c>
     </row>
     <row r="19" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="62"/>
+      <c r="D19" s="86"/>
       <c r="E19" s="11">
         <v>41421</v>
       </c>
@@ -2355,11 +2594,11 @@
       </c>
     </row>
     <row r="20" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="46"/>
-      <c r="C20" s="58" t="s">
+      <c r="B20" s="70"/>
+      <c r="C20" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="63"/>
+      <c r="D20" s="87"/>
       <c r="E20" s="4">
         <v>26094</v>
       </c>
@@ -2455,11 +2694,11 @@
       </c>
     </row>
     <row r="21" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="46"/>
-      <c r="C21" s="48" t="s">
+      <c r="B21" s="70"/>
+      <c r="C21" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="62"/>
+      <c r="D21" s="86"/>
       <c r="E21" s="4">
         <v>15331</v>
       </c>
@@ -2555,11 +2794,11 @@
       </c>
     </row>
     <row r="22" spans="2:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="47"/>
-      <c r="C22" s="50" t="s">
+      <c r="B22" s="71"/>
+      <c r="C22" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="64"/>
+      <c r="D22" s="88"/>
       <c r="E22" s="6">
         <v>1107273</v>
       </c>
@@ -2656,350 +2895,345 @@
     </row>
     <row r="35" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="40" t="s">
+      <c r="E36" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="41"/>
-      <c r="J36" s="41"/>
-      <c r="K36" s="41"/>
-      <c r="L36" s="41"/>
-      <c r="M36" s="41"/>
-      <c r="N36" s="41"/>
-      <c r="O36" s="41"/>
-      <c r="P36" s="41"/>
-      <c r="Q36" s="41"/>
-      <c r="R36" s="41"/>
-      <c r="S36" s="41"/>
-      <c r="T36" s="41"/>
-      <c r="U36" s="41"/>
-      <c r="V36" s="41"/>
-      <c r="W36" s="41"/>
-      <c r="X36" s="41"/>
-      <c r="Y36" s="41"/>
-      <c r="Z36" s="41"/>
-      <c r="AA36" s="41"/>
-      <c r="AB36" s="41"/>
-      <c r="AC36" s="41"/>
-      <c r="AD36" s="41"/>
-      <c r="AE36" s="41"/>
-      <c r="AF36" s="41"/>
-      <c r="AG36" s="41"/>
-      <c r="AH36" s="41"/>
-      <c r="AI36" s="41"/>
-      <c r="AJ36" s="41"/>
-      <c r="AK36" s="41"/>
-      <c r="AL36" s="41"/>
-      <c r="AM36" s="41"/>
-      <c r="AN36" s="41"/>
-      <c r="AO36" s="41"/>
-      <c r="AP36" s="41"/>
-      <c r="AQ36" s="41"/>
-      <c r="AR36" s="41"/>
-      <c r="AS36" s="41"/>
-      <c r="AT36" s="41"/>
-      <c r="AU36" s="41"/>
-      <c r="AV36" s="42"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="65"/>
+      <c r="J36" s="65"/>
+      <c r="K36" s="65"/>
+      <c r="L36" s="65"/>
+      <c r="M36" s="65"/>
+      <c r="N36" s="65"/>
+      <c r="O36" s="65"/>
+      <c r="P36" s="65"/>
+      <c r="Q36" s="65"/>
+      <c r="R36" s="65"/>
+      <c r="S36" s="65"/>
+      <c r="T36" s="65"/>
+      <c r="U36" s="65"/>
+      <c r="V36" s="65"/>
+      <c r="W36" s="65"/>
+      <c r="X36" s="65"/>
+      <c r="Y36" s="65"/>
+      <c r="Z36" s="65"/>
+      <c r="AA36" s="65"/>
+      <c r="AB36" s="65"/>
+      <c r="AC36" s="65"/>
+      <c r="AD36" s="65"/>
+      <c r="AE36" s="65"/>
+      <c r="AF36" s="65"/>
+      <c r="AG36" s="65"/>
+      <c r="AH36" s="65"/>
+      <c r="AI36" s="65"/>
+      <c r="AJ36" s="65"/>
+      <c r="AK36" s="65"/>
+      <c r="AL36" s="65"/>
+      <c r="AM36" s="65"/>
+      <c r="AN36" s="65"/>
+      <c r="AO36" s="65"/>
+      <c r="AP36" s="65"/>
+      <c r="AQ36" s="65"/>
+      <c r="AR36" s="65"/>
+      <c r="AS36" s="65"/>
+      <c r="AT36" s="65"/>
+      <c r="AU36" s="65"/>
+      <c r="AV36" s="66"/>
     </row>
     <row r="37" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="56" t="s">
+      <c r="C37" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="61"/>
-      <c r="E37" s="68">
+      <c r="D37" s="85"/>
+      <c r="E37" s="38">
         <v>1</v>
       </c>
-      <c r="F37" s="66">
+      <c r="F37" s="36">
         <v>2</v>
       </c>
-      <c r="G37" s="66">
+      <c r="G37" s="36">
         <v>3</v>
       </c>
-      <c r="H37" s="66">
+      <c r="H37" s="36">
         <v>4</v>
       </c>
-      <c r="I37" s="66">
+      <c r="I37" s="36">
         <v>5</v>
       </c>
-      <c r="J37" s="66">
+      <c r="J37" s="36">
         <v>6</v>
       </c>
-      <c r="K37" s="66">
+      <c r="K37" s="36">
         <v>7</v>
       </c>
-      <c r="L37" s="66">
+      <c r="L37" s="36">
         <v>8</v>
       </c>
-      <c r="M37" s="66">
+      <c r="M37" s="36">
         <v>9</v>
       </c>
-      <c r="N37" s="66">
+      <c r="N37" s="36">
         <v>10</v>
       </c>
-      <c r="O37" s="66">
+      <c r="O37" s="36">
         <v>11</v>
       </c>
-      <c r="P37" s="66">
+      <c r="P37" s="36">
         <v>12</v>
       </c>
-      <c r="Q37" s="66">
+      <c r="Q37" s="36">
         <v>13</v>
       </c>
-      <c r="R37" s="66">
+      <c r="R37" s="36">
         <v>14</v>
       </c>
-      <c r="S37" s="66">
+      <c r="S37" s="36">
         <v>15</v>
       </c>
-      <c r="T37" s="66">
+      <c r="T37" s="36">
         <v>16</v>
       </c>
-      <c r="U37" s="66">
+      <c r="U37" s="36">
         <v>17</v>
       </c>
-      <c r="V37" s="66">
+      <c r="V37" s="36">
         <v>20</v>
       </c>
-      <c r="W37" s="66">
+      <c r="W37" s="36">
         <v>30</v>
       </c>
-      <c r="X37" s="66">
+      <c r="X37" s="36">
         <v>40</v>
       </c>
-      <c r="Y37" s="66">
+      <c r="Y37" s="36">
         <v>50</v>
       </c>
-      <c r="Z37" s="66">
+      <c r="Z37" s="36">
         <v>60</v>
       </c>
-      <c r="AA37" s="66">
+      <c r="AA37" s="36">
         <v>70</v>
       </c>
-      <c r="AB37" s="66">
+      <c r="AB37" s="36">
         <v>80</v>
       </c>
-      <c r="AC37" s="66">
+      <c r="AC37" s="36">
         <v>90</v>
       </c>
-      <c r="AD37" s="66">
+      <c r="AD37" s="36">
         <v>100</v>
       </c>
-      <c r="AE37" s="66">
+      <c r="AE37" s="36">
         <v>120</v>
       </c>
-      <c r="AF37" s="66">
+      <c r="AF37" s="36">
         <v>140</v>
       </c>
-      <c r="AG37" s="66">
+      <c r="AG37" s="36">
         <v>175</v>
       </c>
-      <c r="AH37" s="66">
+      <c r="AH37" s="36">
         <v>200</v>
       </c>
-      <c r="AI37" s="67">
+      <c r="AI37" s="37">
         <v>225</v>
       </c>
-      <c r="AJ37" s="81">
+      <c r="AJ37" s="50">
         <v>250</v>
       </c>
-      <c r="AK37" s="67">
+      <c r="AK37" s="37">
         <v>275</v>
       </c>
-      <c r="AL37" s="73">
+      <c r="AL37" s="43">
         <v>280</v>
       </c>
-      <c r="AM37" s="76">
+      <c r="AM37" s="45">
         <v>285</v>
       </c>
-      <c r="AN37" s="76">
+      <c r="AN37" s="45">
         <v>290</v>
       </c>
-      <c r="AO37" s="76">
+      <c r="AO37" s="45">
         <v>295</v>
       </c>
-      <c r="AP37" s="66">
+      <c r="AP37" s="36">
         <v>300</v>
       </c>
-      <c r="AQ37" s="67">
+      <c r="AQ37" s="37">
         <v>325</v>
       </c>
-      <c r="AR37" s="66">
+      <c r="AR37" s="36">
         <v>350</v>
       </c>
-      <c r="AS37" s="67">
+      <c r="AS37" s="37">
         <v>375</v>
       </c>
-      <c r="AT37" s="66">
+      <c r="AT37" s="36">
         <v>400</v>
       </c>
-      <c r="AU37" s="67">
+      <c r="AU37" s="37">
         <v>425</v>
       </c>
       <c r="AV37" s="18">
         <v>450</v>
       </c>
-      <c r="AW37" s="73"/>
-      <c r="AX37" s="73"/>
-      <c r="AY37" s="73"/>
-      <c r="AZ37" s="73"/>
-      <c r="BA37" s="73"/>
-      <c r="BB37" s="73"/>
+      <c r="AW37" s="43"/>
+      <c r="AX37" s="43"/>
+      <c r="AY37" s="43"/>
+      <c r="AZ37" s="43"/>
+      <c r="BA37" s="43"/>
+      <c r="BB37" s="43"/>
     </row>
     <row r="38" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="45" t="s">
+      <c r="B38" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="48" t="s">
+      <c r="C38" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="62"/>
-      <c r="E38" s="69">
+      <c r="D38" s="86"/>
+      <c r="E38" s="39">
         <v>41768</v>
       </c>
-      <c r="F38" s="70">
+      <c r="F38" s="40">
         <v>20910</v>
       </c>
-      <c r="G38" s="70">
+      <c r="G38" s="40">
         <v>13985</v>
       </c>
-      <c r="H38" s="70">
+      <c r="H38" s="40">
         <v>10483</v>
       </c>
-      <c r="I38" s="70">
+      <c r="I38" s="40">
         <v>8404</v>
       </c>
-      <c r="J38" s="70">
+      <c r="J38" s="40">
         <v>7023</v>
       </c>
-      <c r="K38" s="70">
+      <c r="K38" s="40">
         <v>6030</v>
       </c>
-      <c r="L38" s="70">
+      <c r="L38" s="40">
         <v>5270</v>
       </c>
-      <c r="M38" s="70">
+      <c r="M38" s="40">
         <v>4698</v>
       </c>
-      <c r="N38" s="70">
+      <c r="N38" s="40">
         <v>4223</v>
       </c>
-      <c r="O38" s="70">
+      <c r="O38" s="40">
         <v>3862</v>
       </c>
-      <c r="P38" s="70">
+      <c r="P38" s="40">
         <v>3542</v>
       </c>
-      <c r="Q38" s="70">
+      <c r="Q38" s="40">
         <v>3270</v>
       </c>
-      <c r="R38" s="70">
+      <c r="R38" s="40">
         <v>3059</v>
       </c>
-      <c r="S38" s="70">
+      <c r="S38" s="40">
         <v>2831</v>
       </c>
-      <c r="T38" s="70">
+      <c r="T38" s="40">
         <v>2597</v>
       </c>
-      <c r="U38" s="70">
+      <c r="U38" s="40">
         <v>2538</v>
       </c>
-      <c r="V38" s="70">
+      <c r="V38" s="40">
         <v>2134</v>
       </c>
-      <c r="W38" s="70">
+      <c r="W38" s="40">
         <v>1436</v>
       </c>
-      <c r="X38" s="70">
+      <c r="X38" s="40">
         <v>1085</v>
       </c>
-      <c r="Y38" s="70">
+      <c r="Y38" s="40">
         <v>930</v>
       </c>
-      <c r="Z38" s="70">
+      <c r="Z38" s="40">
         <v>794</v>
       </c>
-      <c r="AA38" s="70">
+      <c r="AA38" s="40">
         <v>753</v>
       </c>
-      <c r="AB38" s="70">
+      <c r="AB38" s="40">
         <v>659</v>
       </c>
-      <c r="AC38" s="70">
+      <c r="AC38" s="40">
         <v>611</v>
       </c>
-      <c r="AD38" s="70">
+      <c r="AD38" s="40">
         <v>574</v>
       </c>
-      <c r="AE38" s="70">
+      <c r="AE38" s="40">
         <v>524</v>
       </c>
-      <c r="AF38" s="70">
+      <c r="AF38" s="40">
         <v>482</v>
       </c>
-      <c r="AG38" s="70">
+      <c r="AG38" s="40">
         <v>428</v>
       </c>
-      <c r="AH38" s="70">
+      <c r="AH38" s="40">
         <v>410</v>
       </c>
-      <c r="AI38" s="70">
+      <c r="AI38" s="40">
         <v>387</v>
       </c>
-      <c r="AJ38" s="82">
+      <c r="AJ38" s="51">
         <v>391</v>
       </c>
-      <c r="AK38" s="71">
+      <c r="AK38" s="41">
         <v>392</v>
       </c>
-      <c r="AL38" s="76">
+      <c r="AL38" s="45">
         <v>406</v>
       </c>
-      <c r="AM38" s="71">
+      <c r="AM38" s="41">
         <v>402</v>
       </c>
-      <c r="AN38" s="71">
+      <c r="AN38" s="41">
         <v>403</v>
       </c>
-      <c r="AO38" s="71">
+      <c r="AO38" s="41">
         <v>404</v>
       </c>
-      <c r="AP38" s="71">
+      <c r="AP38" s="41">
         <v>404</v>
       </c>
-      <c r="AQ38" s="71">
+      <c r="AQ38" s="41">
         <v>402</v>
       </c>
-      <c r="AR38" s="71">
+      <c r="AR38" s="41">
         <v>405</v>
       </c>
-      <c r="AS38" s="71">
+      <c r="AS38" s="41">
         <v>408</v>
       </c>
-      <c r="AT38" s="71">
+      <c r="AT38" s="41">
         <v>407</v>
       </c>
-      <c r="AU38" s="71">
+      <c r="AU38" s="41">
         <v>410</v>
       </c>
-      <c r="AV38" s="72">
+      <c r="AV38" s="42">
         <v>410</v>
       </c>
-      <c r="AW38" s="74"/>
-      <c r="AX38" s="75"/>
-      <c r="AY38" s="75"/>
-      <c r="AZ38" s="75"/>
-      <c r="BA38" s="75"/>
-      <c r="BB38" s="75"/>
+      <c r="AW38" s="44"/>
     </row>
     <row r="39" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="46"/>
-      <c r="C39" s="58" t="s">
+      <c r="B39" s="70"/>
+      <c r="C39" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="D39" s="63"/>
+      <c r="D39" s="87"/>
       <c r="E39" s="4">
         <v>23012</v>
       </c>
@@ -3093,7 +3327,7 @@
       <c r="AI39" s="1">
         <v>244</v>
       </c>
-      <c r="AJ39" s="83">
+      <c r="AJ39" s="52">
         <v>245</v>
       </c>
       <c r="AK39" s="26">
@@ -3132,19 +3366,14 @@
       <c r="AV39" s="31">
         <v>265</v>
       </c>
-      <c r="AW39" s="74"/>
-      <c r="AX39" s="75"/>
-      <c r="AY39" s="75"/>
-      <c r="AZ39" s="75"/>
-      <c r="BA39" s="75"/>
-      <c r="BB39" s="75"/>
+      <c r="AW39" s="44"/>
     </row>
     <row r="40" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="46"/>
-      <c r="C40" s="48" t="s">
+      <c r="B40" s="70"/>
+      <c r="C40" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="62"/>
+      <c r="D40" s="86"/>
       <c r="E40" s="4">
         <v>13545</v>
       </c>
@@ -3238,7 +3467,7 @@
       <c r="AI40" s="1">
         <v>166</v>
       </c>
-      <c r="AJ40" s="83">
+      <c r="AJ40" s="52">
         <v>165</v>
       </c>
       <c r="AK40" s="26">
@@ -3277,19 +3506,14 @@
       <c r="AV40" s="31">
         <v>171</v>
       </c>
-      <c r="AW40" s="74"/>
-      <c r="AX40" s="75"/>
-      <c r="AY40" s="75"/>
-      <c r="AZ40" s="75"/>
-      <c r="BA40" s="75"/>
-      <c r="BB40" s="75"/>
+      <c r="AW40" s="44"/>
     </row>
     <row r="41" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="47"/>
-      <c r="C41" s="50" t="s">
+      <c r="B41" s="71"/>
+      <c r="C41" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="64"/>
+      <c r="D41" s="88"/>
       <c r="E41" s="6">
         <v>1076471</v>
       </c>
@@ -3383,7 +3607,7 @@
       <c r="AI41" s="7">
         <v>8955</v>
       </c>
-      <c r="AJ41" s="84">
+      <c r="AJ41" s="53">
         <v>8926</v>
       </c>
       <c r="AK41" s="27">
@@ -3422,59 +3646,54 @@
       <c r="AV41" s="32">
         <v>9533</v>
       </c>
-      <c r="AW41" s="74"/>
-      <c r="AX41" s="75"/>
-      <c r="AY41" s="75"/>
-      <c r="AZ41" s="75"/>
-      <c r="BA41" s="75"/>
-      <c r="BB41" s="75"/>
+      <c r="AW41" s="44"/>
     </row>
     <row r="43" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="65"/>
-      <c r="D43" s="65"/>
-      <c r="E43" s="65"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
     </row>
     <row r="44" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="56" t="s">
+      <c r="C44" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="D44" s="61"/>
+      <c r="D44" s="85"/>
       <c r="E44" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="45" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="48" t="s">
+      <c r="C45" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="62"/>
+      <c r="D45" s="86"/>
       <c r="E45" s="19">
         <v>28218</v>
       </c>
     </row>
     <row r="46" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="58" t="s">
+      <c r="C46" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="63"/>
+      <c r="D46" s="87"/>
       <c r="E46" s="20">
         <v>14757</v>
       </c>
     </row>
     <row r="47" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C47" s="48" t="s">
+      <c r="C47" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="62"/>
+      <c r="D47" s="86"/>
       <c r="E47" s="20">
         <v>8108</v>
       </c>
     </row>
     <row r="48" spans="2:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="50" t="s">
+      <c r="C48" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D48" s="64"/>
+      <c r="D48" s="88"/>
       <c r="E48" s="21">
         <v>898369</v>
       </c>
@@ -3501,7 +3720,7 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="E3:AP4"/>
     <mergeCell ref="E17:AI17"/>
-    <mergeCell ref="AQ5:AQ6"/>
+    <mergeCell ref="AM5:AM6"/>
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
@@ -3512,9 +3731,3002 @@
     <mergeCell ref="E5:O6"/>
     <mergeCell ref="P5:Z6"/>
     <mergeCell ref="AA5:AK6"/>
-    <mergeCell ref="AP5:AP6"/>
+    <mergeCell ref="AL5:AL6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBD9BA9-E8F5-498B-A25F-8614A381C5CE}">
+  <dimension ref="C5:CZ46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="P9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL51" sqref="AL51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="3:104" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="3:104" x14ac:dyDescent="0.25">
+      <c r="F6" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="59"/>
+      <c r="Q6" s="59"/>
+      <c r="R6" s="59"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
+      <c r="U6" s="59"/>
+      <c r="V6" s="59"/>
+      <c r="W6" s="59"/>
+      <c r="X6" s="59"/>
+      <c r="Y6" s="59"/>
+      <c r="Z6" s="59"/>
+      <c r="AA6" s="59"/>
+      <c r="AB6" s="59"/>
+      <c r="AC6" s="59"/>
+      <c r="AD6" s="59"/>
+      <c r="AE6" s="59"/>
+      <c r="AF6" s="59"/>
+      <c r="AG6" s="59"/>
+      <c r="AH6" s="59"/>
+      <c r="AI6" s="59"/>
+      <c r="AJ6" s="59"/>
+      <c r="AK6" s="59"/>
+      <c r="AL6" s="60"/>
+      <c r="AM6" s="15"/>
+      <c r="AN6" s="15"/>
+      <c r="AO6" s="15"/>
+      <c r="AP6" s="15"/>
+      <c r="AQ6" s="15"/>
+      <c r="AR6" s="15"/>
+      <c r="AS6" s="15"/>
+      <c r="AT6" s="15"/>
+      <c r="AU6" s="15"/>
+      <c r="AV6" s="15"/>
+      <c r="AW6" s="15"/>
+      <c r="AX6" s="15"/>
+      <c r="AY6" s="15"/>
+      <c r="AZ6" s="15"/>
+      <c r="BA6" s="15"/>
+      <c r="BB6" s="15"/>
+      <c r="BC6" s="15"/>
+      <c r="BD6" s="15"/>
+      <c r="BE6" s="15"/>
+      <c r="BF6" s="15"/>
+      <c r="BG6" s="15"/>
+      <c r="BH6" s="15"/>
+      <c r="BI6" s="15"/>
+      <c r="BJ6" s="15"/>
+      <c r="BK6" s="15"/>
+      <c r="BL6" s="15"/>
+      <c r="BM6" s="15"/>
+      <c r="BN6" s="15"/>
+      <c r="BO6" s="15"/>
+      <c r="BP6" s="15"/>
+      <c r="BQ6" s="15"/>
+      <c r="BR6" s="15"/>
+      <c r="BS6" s="15"/>
+      <c r="BT6" s="15"/>
+      <c r="BU6" s="15"/>
+      <c r="BV6" s="15"/>
+      <c r="BW6" s="15"/>
+      <c r="BX6" s="15"/>
+      <c r="BY6" s="15"/>
+      <c r="BZ6" s="15"/>
+      <c r="CA6" s="15"/>
+      <c r="CB6" s="15"/>
+      <c r="CC6" s="15"/>
+      <c r="CD6" s="15"/>
+      <c r="CE6" s="15"/>
+      <c r="CF6" s="15"/>
+      <c r="CG6" s="15"/>
+      <c r="CH6" s="15"/>
+      <c r="CI6" s="15"/>
+      <c r="CJ6" s="15"/>
+      <c r="CK6" s="15"/>
+      <c r="CL6" s="15"/>
+      <c r="CM6" s="15"/>
+      <c r="CN6" s="15"/>
+      <c r="CO6" s="15"/>
+      <c r="CP6" s="15"/>
+      <c r="CQ6" s="15"/>
+      <c r="CR6" s="15"/>
+      <c r="CS6" s="15"/>
+      <c r="CT6" s="15"/>
+      <c r="CU6" s="15"/>
+      <c r="CV6" s="15"/>
+      <c r="CW6" s="15"/>
+      <c r="CX6" s="15"/>
+      <c r="CY6" s="15"/>
+      <c r="CZ6" s="15"/>
+    </row>
+    <row r="7" spans="3:104" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="61"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="62"/>
+      <c r="O7" s="62"/>
+      <c r="P7" s="62"/>
+      <c r="Q7" s="62"/>
+      <c r="R7" s="62"/>
+      <c r="S7" s="62"/>
+      <c r="T7" s="62"/>
+      <c r="U7" s="62"/>
+      <c r="V7" s="62"/>
+      <c r="W7" s="62"/>
+      <c r="X7" s="62"/>
+      <c r="Y7" s="62"/>
+      <c r="Z7" s="62"/>
+      <c r="AA7" s="62"/>
+      <c r="AB7" s="62"/>
+      <c r="AC7" s="62"/>
+      <c r="AD7" s="62"/>
+      <c r="AE7" s="62"/>
+      <c r="AF7" s="62"/>
+      <c r="AG7" s="62"/>
+      <c r="AH7" s="62"/>
+      <c r="AI7" s="62"/>
+      <c r="AJ7" s="62"/>
+      <c r="AK7" s="62"/>
+      <c r="AL7" s="63"/>
+      <c r="AM7" s="15"/>
+      <c r="AN7" s="15"/>
+      <c r="AO7" s="15"/>
+      <c r="AP7" s="15"/>
+      <c r="AQ7" s="15"/>
+      <c r="AR7" s="15"/>
+      <c r="AS7" s="15"/>
+      <c r="AT7" s="15"/>
+      <c r="AU7" s="15"/>
+      <c r="AV7" s="15"/>
+      <c r="AW7" s="15"/>
+      <c r="AX7" s="15"/>
+      <c r="AY7" s="15"/>
+      <c r="AZ7" s="15"/>
+      <c r="BA7" s="15"/>
+      <c r="BB7" s="15"/>
+      <c r="BC7" s="15"/>
+      <c r="BD7" s="15"/>
+      <c r="BE7" s="15"/>
+      <c r="BF7" s="15"/>
+      <c r="BG7" s="15"/>
+      <c r="BH7" s="15"/>
+      <c r="BI7" s="15"/>
+      <c r="BJ7" s="15"/>
+      <c r="BK7" s="15"/>
+      <c r="BL7" s="15"/>
+      <c r="BM7" s="15"/>
+      <c r="BN7" s="15"/>
+      <c r="BO7" s="15"/>
+      <c r="BP7" s="15"/>
+      <c r="BQ7" s="15"/>
+      <c r="BR7" s="15"/>
+      <c r="BS7" s="15"/>
+      <c r="BT7" s="15"/>
+      <c r="BU7" s="15"/>
+      <c r="BV7" s="15"/>
+      <c r="BW7" s="15"/>
+      <c r="BX7" s="15"/>
+      <c r="BY7" s="15"/>
+      <c r="BZ7" s="15"/>
+      <c r="CA7" s="15"/>
+      <c r="CB7" s="15"/>
+      <c r="CC7" s="15"/>
+      <c r="CD7" s="15"/>
+      <c r="CE7" s="15"/>
+      <c r="CF7" s="15"/>
+      <c r="CG7" s="15"/>
+      <c r="CH7" s="15"/>
+      <c r="CI7" s="15"/>
+      <c r="CJ7" s="15"/>
+      <c r="CK7" s="15"/>
+      <c r="CL7" s="15"/>
+      <c r="CM7" s="15"/>
+      <c r="CN7" s="15"/>
+      <c r="CO7" s="15"/>
+      <c r="CP7" s="15"/>
+      <c r="CQ7" s="15"/>
+      <c r="CR7" s="15"/>
+      <c r="CS7" s="15"/>
+      <c r="CT7" s="15"/>
+      <c r="CU7" s="15"/>
+      <c r="CV7" s="15"/>
+      <c r="CW7" s="15"/>
+      <c r="CX7" s="15"/>
+      <c r="CY7" s="15"/>
+      <c r="CZ7" s="15"/>
+    </row>
+    <row r="8" spans="3:104" x14ac:dyDescent="0.25">
+      <c r="D8" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="77"/>
+      <c r="F8" s="89" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="90"/>
+      <c r="N8" s="90"/>
+      <c r="O8" s="90"/>
+      <c r="P8" s="90"/>
+      <c r="Q8" s="90"/>
+      <c r="R8" s="90"/>
+      <c r="S8" s="90"/>
+      <c r="T8" s="90"/>
+      <c r="U8" s="90"/>
+      <c r="V8" s="90"/>
+      <c r="W8" s="90"/>
+      <c r="X8" s="90"/>
+      <c r="Y8" s="90"/>
+      <c r="Z8" s="90"/>
+      <c r="AA8" s="90"/>
+      <c r="AB8" s="90"/>
+      <c r="AC8" s="90"/>
+      <c r="AD8" s="90"/>
+      <c r="AE8" s="90"/>
+      <c r="AF8" s="90"/>
+      <c r="AG8" s="90"/>
+      <c r="AH8" s="90"/>
+      <c r="AI8" s="90"/>
+      <c r="AJ8" s="90"/>
+      <c r="AK8" s="90"/>
+      <c r="AL8" s="91"/>
+    </row>
+    <row r="9" spans="3:104" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="78"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="93"/>
+      <c r="H9" s="93"/>
+      <c r="I9" s="93"/>
+      <c r="J9" s="93"/>
+      <c r="K9" s="93"/>
+      <c r="L9" s="93"/>
+      <c r="M9" s="93"/>
+      <c r="N9" s="93"/>
+      <c r="O9" s="93"/>
+      <c r="P9" s="93"/>
+      <c r="Q9" s="93"/>
+      <c r="R9" s="93"/>
+      <c r="S9" s="93"/>
+      <c r="T9" s="93"/>
+      <c r="U9" s="93"/>
+      <c r="V9" s="93"/>
+      <c r="W9" s="93"/>
+      <c r="X9" s="93"/>
+      <c r="Y9" s="93"/>
+      <c r="Z9" s="93"/>
+      <c r="AA9" s="93"/>
+      <c r="AB9" s="93"/>
+      <c r="AC9" s="93"/>
+      <c r="AD9" s="93"/>
+      <c r="AE9" s="93"/>
+      <c r="AF9" s="93"/>
+      <c r="AG9" s="93"/>
+      <c r="AH9" s="93"/>
+      <c r="AI9" s="93"/>
+      <c r="AJ9" s="93"/>
+      <c r="AK9" s="93"/>
+      <c r="AL9" s="94"/>
+    </row>
+    <row r="10" spans="3:104" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="80" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="81"/>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="16">
+        <v>2</v>
+      </c>
+      <c r="H10" s="16">
+        <v>4</v>
+      </c>
+      <c r="I10" s="14">
+        <v>6</v>
+      </c>
+      <c r="J10" s="14">
+        <v>8</v>
+      </c>
+      <c r="K10" s="14">
+        <v>10</v>
+      </c>
+      <c r="L10" s="14">
+        <v>12</v>
+      </c>
+      <c r="M10" s="14">
+        <v>14</v>
+      </c>
+      <c r="N10" s="14">
+        <v>16</v>
+      </c>
+      <c r="O10" s="14">
+        <v>18</v>
+      </c>
+      <c r="P10" s="14">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="14">
+        <v>22</v>
+      </c>
+      <c r="R10" s="14">
+        <v>24</v>
+      </c>
+      <c r="S10" s="14">
+        <v>26</v>
+      </c>
+      <c r="T10" s="14">
+        <v>28</v>
+      </c>
+      <c r="U10" s="14">
+        <v>32</v>
+      </c>
+      <c r="V10" s="14">
+        <v>36</v>
+      </c>
+      <c r="W10" s="14">
+        <v>40</v>
+      </c>
+      <c r="X10" s="14">
+        <v>44</v>
+      </c>
+      <c r="Y10" s="14">
+        <v>48</v>
+      </c>
+      <c r="Z10" s="34">
+        <v>52</v>
+      </c>
+      <c r="AA10" s="34">
+        <v>56</v>
+      </c>
+      <c r="AB10" s="34">
+        <v>60</v>
+      </c>
+      <c r="AC10" s="34">
+        <v>64</v>
+      </c>
+      <c r="AD10" s="34">
+        <v>80</v>
+      </c>
+      <c r="AE10" s="34">
+        <v>96</v>
+      </c>
+      <c r="AF10" s="34">
+        <v>112</v>
+      </c>
+      <c r="AG10" s="34">
+        <v>128</v>
+      </c>
+      <c r="AH10" s="34">
+        <v>144</v>
+      </c>
+      <c r="AI10" s="34">
+        <v>160</v>
+      </c>
+      <c r="AJ10" s="34">
+        <v>176</v>
+      </c>
+      <c r="AK10" s="34">
+        <v>192</v>
+      </c>
+      <c r="AL10" s="3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="3:104" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="73"/>
+      <c r="F11" s="11">
+        <v>9559</v>
+      </c>
+      <c r="G11" s="17">
+        <v>9568</v>
+      </c>
+      <c r="H11" s="17">
+        <v>9559</v>
+      </c>
+      <c r="I11" s="12">
+        <v>9568</v>
+      </c>
+      <c r="J11" s="12">
+        <v>9560</v>
+      </c>
+      <c r="K11" s="12">
+        <v>9560</v>
+      </c>
+      <c r="L11" s="12">
+        <v>9562</v>
+      </c>
+      <c r="M11" s="12">
+        <v>9574</v>
+      </c>
+      <c r="N11" s="12">
+        <v>9589</v>
+      </c>
+      <c r="O11" s="12">
+        <v>9564</v>
+      </c>
+      <c r="P11" s="12">
+        <v>9564</v>
+      </c>
+      <c r="Q11" s="12">
+        <v>9582</v>
+      </c>
+      <c r="R11" s="12">
+        <v>9565</v>
+      </c>
+      <c r="S11" s="12">
+        <v>9588</v>
+      </c>
+      <c r="T11" s="12">
+        <v>9562</v>
+      </c>
+      <c r="U11" s="12">
+        <v>9571</v>
+      </c>
+      <c r="V11" s="12">
+        <v>9599</v>
+      </c>
+      <c r="W11" s="12">
+        <v>9564</v>
+      </c>
+      <c r="X11" s="12">
+        <v>9564</v>
+      </c>
+      <c r="Y11" s="12">
+        <v>9592</v>
+      </c>
+      <c r="Z11" s="54">
+        <v>9563</v>
+      </c>
+      <c r="AA11" s="54">
+        <v>9590</v>
+      </c>
+      <c r="AB11" s="54">
+        <v>9594</v>
+      </c>
+      <c r="AC11" s="54">
+        <v>9598</v>
+      </c>
+      <c r="AD11" s="54">
+        <v>9738</v>
+      </c>
+      <c r="AE11" s="54">
+        <v>9657</v>
+      </c>
+      <c r="AF11" s="54">
+        <v>9673</v>
+      </c>
+      <c r="AG11" s="54">
+        <v>9633</v>
+      </c>
+      <c r="AH11" s="54">
+        <v>10035</v>
+      </c>
+      <c r="AI11" s="54">
+        <v>10231</v>
+      </c>
+      <c r="AJ11" s="54">
+        <v>9695</v>
+      </c>
+      <c r="AK11" s="54">
+        <v>9939</v>
+      </c>
+      <c r="AL11" s="13">
+        <v>10452</v>
+      </c>
+    </row>
+    <row r="12" spans="3:104" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="70"/>
+      <c r="D12" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="83"/>
+      <c r="F12" s="4">
+        <v>1593</v>
+      </c>
+      <c r="G12" s="9">
+        <v>1590</v>
+      </c>
+      <c r="H12" s="9">
+        <v>1590</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1588</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1590</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1591</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1595</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1591</v>
+      </c>
+      <c r="N12" s="1">
+        <v>1592</v>
+      </c>
+      <c r="O12" s="1">
+        <v>1592</v>
+      </c>
+      <c r="P12" s="1">
+        <v>1598</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>1589</v>
+      </c>
+      <c r="R12" s="1">
+        <v>1593</v>
+      </c>
+      <c r="S12" s="1">
+        <v>1602</v>
+      </c>
+      <c r="T12" s="1">
+        <v>1591</v>
+      </c>
+      <c r="U12" s="1">
+        <v>1608</v>
+      </c>
+      <c r="V12" s="1">
+        <v>1592</v>
+      </c>
+      <c r="W12" s="1">
+        <v>1593</v>
+      </c>
+      <c r="X12" s="1">
+        <v>1610</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>1591</v>
+      </c>
+      <c r="Z12" s="55">
+        <v>1592</v>
+      </c>
+      <c r="AA12" s="55">
+        <v>1591</v>
+      </c>
+      <c r="AB12" s="55">
+        <v>1596</v>
+      </c>
+      <c r="AC12" s="55">
+        <v>1593</v>
+      </c>
+      <c r="AD12" s="55">
+        <v>1593</v>
+      </c>
+      <c r="AE12" s="55">
+        <v>1594</v>
+      </c>
+      <c r="AF12" s="55">
+        <v>1601</v>
+      </c>
+      <c r="AG12" s="55">
+        <v>1597</v>
+      </c>
+      <c r="AH12" s="55">
+        <v>1594</v>
+      </c>
+      <c r="AI12" s="55">
+        <v>1604</v>
+      </c>
+      <c r="AJ12" s="55">
+        <v>1613</v>
+      </c>
+      <c r="AK12" s="55">
+        <v>1591</v>
+      </c>
+      <c r="AL12" s="5">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="13" spans="3:104" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="70"/>
+      <c r="D13" s="72" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="73"/>
+      <c r="F13" s="4">
+        <v>2795</v>
+      </c>
+      <c r="G13" s="9">
+        <v>2798</v>
+      </c>
+      <c r="H13" s="9">
+        <v>2797</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2799</v>
+      </c>
+      <c r="J13" s="1">
+        <v>2798</v>
+      </c>
+      <c r="K13" s="1">
+        <v>2810</v>
+      </c>
+      <c r="L13" s="1">
+        <v>2804</v>
+      </c>
+      <c r="M13" s="1">
+        <v>2800</v>
+      </c>
+      <c r="N13" s="1">
+        <v>2798</v>
+      </c>
+      <c r="O13" s="1">
+        <v>2801</v>
+      </c>
+      <c r="P13" s="1">
+        <v>2799</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>2801</v>
+      </c>
+      <c r="R13" s="1">
+        <v>2800</v>
+      </c>
+      <c r="S13" s="1">
+        <v>2812</v>
+      </c>
+      <c r="T13" s="1">
+        <v>2812</v>
+      </c>
+      <c r="U13" s="1">
+        <v>2801</v>
+      </c>
+      <c r="V13" s="1">
+        <v>2795</v>
+      </c>
+      <c r="W13" s="1">
+        <v>2798</v>
+      </c>
+      <c r="X13" s="1">
+        <v>2796</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>2808</v>
+      </c>
+      <c r="Z13" s="55">
+        <v>2802</v>
+      </c>
+      <c r="AA13" s="55">
+        <v>2802</v>
+      </c>
+      <c r="AB13" s="55">
+        <v>2807</v>
+      </c>
+      <c r="AC13" s="55">
+        <v>2802</v>
+      </c>
+      <c r="AD13" s="55">
+        <v>2806</v>
+      </c>
+      <c r="AE13" s="55">
+        <v>2836</v>
+      </c>
+      <c r="AF13" s="55">
+        <v>2845</v>
+      </c>
+      <c r="AG13" s="55">
+        <v>2841</v>
+      </c>
+      <c r="AH13" s="55">
+        <v>2838</v>
+      </c>
+      <c r="AI13" s="55">
+        <v>3317</v>
+      </c>
+      <c r="AJ13" s="55">
+        <v>3427</v>
+      </c>
+      <c r="AK13" s="55">
+        <v>3690</v>
+      </c>
+      <c r="AL13" s="5">
+        <v>3833</v>
+      </c>
+    </row>
+    <row r="14" spans="3:104" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="71"/>
+      <c r="D14" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="75"/>
+      <c r="F14" s="6">
+        <v>250952</v>
+      </c>
+      <c r="G14" s="10">
+        <v>250422</v>
+      </c>
+      <c r="H14" s="10">
+        <v>250692</v>
+      </c>
+      <c r="I14" s="7">
+        <v>250377</v>
+      </c>
+      <c r="J14" s="7">
+        <v>250430</v>
+      </c>
+      <c r="K14" s="7">
+        <v>250696</v>
+      </c>
+      <c r="L14" s="7">
+        <v>250388</v>
+      </c>
+      <c r="M14" s="7">
+        <v>250356</v>
+      </c>
+      <c r="N14" s="7">
+        <v>250663</v>
+      </c>
+      <c r="O14" s="7">
+        <v>250462</v>
+      </c>
+      <c r="P14" s="7">
+        <v>250898</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>250427</v>
+      </c>
+      <c r="R14" s="7">
+        <v>250384</v>
+      </c>
+      <c r="S14" s="7">
+        <v>250548</v>
+      </c>
+      <c r="T14" s="7">
+        <v>250441</v>
+      </c>
+      <c r="U14" s="7">
+        <v>250924</v>
+      </c>
+      <c r="V14" s="7">
+        <v>250497</v>
+      </c>
+      <c r="W14" s="7">
+        <v>250427</v>
+      </c>
+      <c r="X14" s="7">
+        <v>250660</v>
+      </c>
+      <c r="Y14" s="7">
+        <v>250844</v>
+      </c>
+      <c r="Z14" s="56">
+        <v>250809</v>
+      </c>
+      <c r="AA14" s="56">
+        <v>250508</v>
+      </c>
+      <c r="AB14" s="56">
+        <v>250759</v>
+      </c>
+      <c r="AC14" s="56">
+        <v>251055</v>
+      </c>
+      <c r="AD14" s="56">
+        <v>250693</v>
+      </c>
+      <c r="AE14" s="56">
+        <v>251854</v>
+      </c>
+      <c r="AF14" s="56">
+        <v>253054</v>
+      </c>
+      <c r="AG14" s="56">
+        <v>251379</v>
+      </c>
+      <c r="AH14" s="56">
+        <v>252488</v>
+      </c>
+      <c r="AI14" s="56">
+        <v>251913</v>
+      </c>
+      <c r="AJ14" s="56">
+        <v>253845</v>
+      </c>
+      <c r="AK14" s="56">
+        <v>255274</v>
+      </c>
+      <c r="AL14" s="8">
+        <v>251305</v>
+      </c>
+    </row>
+    <row r="15" spans="3:104" x14ac:dyDescent="0.25">
+      <c r="F15" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="96"/>
+      <c r="H15" s="96"/>
+      <c r="I15" s="96"/>
+      <c r="J15" s="96"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="96"/>
+      <c r="M15" s="96"/>
+      <c r="N15" s="96"/>
+      <c r="O15" s="96"/>
+      <c r="P15" s="96"/>
+      <c r="Q15" s="96"/>
+      <c r="R15" s="96"/>
+      <c r="S15" s="96"/>
+      <c r="T15" s="96"/>
+      <c r="U15" s="96"/>
+      <c r="V15" s="96"/>
+      <c r="W15" s="96"/>
+      <c r="X15" s="96"/>
+      <c r="Y15" s="96"/>
+      <c r="Z15" s="96"/>
+      <c r="AA15" s="96"/>
+      <c r="AB15" s="96"/>
+      <c r="AC15" s="96"/>
+      <c r="AD15" s="96"/>
+      <c r="AE15" s="96"/>
+      <c r="AF15" s="96"/>
+      <c r="AG15" s="96"/>
+      <c r="AH15" s="96"/>
+      <c r="AI15" s="96"/>
+      <c r="AJ15" s="96"/>
+      <c r="AK15" s="96"/>
+      <c r="AL15" s="97"/>
+    </row>
+    <row r="16" spans="3:104" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="98"/>
+      <c r="G16" s="99"/>
+      <c r="H16" s="99"/>
+      <c r="I16" s="99"/>
+      <c r="J16" s="99"/>
+      <c r="K16" s="99"/>
+      <c r="L16" s="99"/>
+      <c r="M16" s="99"/>
+      <c r="N16" s="99"/>
+      <c r="O16" s="99"/>
+      <c r="P16" s="99"/>
+      <c r="Q16" s="99"/>
+      <c r="R16" s="99"/>
+      <c r="S16" s="99"/>
+      <c r="T16" s="99"/>
+      <c r="U16" s="99"/>
+      <c r="V16" s="99"/>
+      <c r="W16" s="99"/>
+      <c r="X16" s="99"/>
+      <c r="Y16" s="99"/>
+      <c r="Z16" s="99"/>
+      <c r="AA16" s="99"/>
+      <c r="AB16" s="99"/>
+      <c r="AC16" s="99"/>
+      <c r="AD16" s="99"/>
+      <c r="AE16" s="99"/>
+      <c r="AF16" s="99"/>
+      <c r="AG16" s="99"/>
+      <c r="AH16" s="99"/>
+      <c r="AI16" s="99"/>
+      <c r="AJ16" s="99"/>
+      <c r="AK16" s="99"/>
+      <c r="AL16" s="100"/>
+    </row>
+    <row r="17" spans="3:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="80" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="81"/>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+      <c r="G17" s="16">
+        <v>2</v>
+      </c>
+      <c r="H17" s="16">
+        <v>4</v>
+      </c>
+      <c r="I17" s="14">
+        <v>6</v>
+      </c>
+      <c r="J17" s="14">
+        <v>8</v>
+      </c>
+      <c r="K17" s="14">
+        <v>10</v>
+      </c>
+      <c r="L17" s="14">
+        <v>12</v>
+      </c>
+      <c r="M17" s="14">
+        <v>14</v>
+      </c>
+      <c r="N17" s="14">
+        <v>16</v>
+      </c>
+      <c r="O17" s="14">
+        <v>18</v>
+      </c>
+      <c r="P17" s="14">
+        <v>20</v>
+      </c>
+      <c r="Q17" s="14">
+        <v>22</v>
+      </c>
+      <c r="R17" s="14">
+        <v>24</v>
+      </c>
+      <c r="S17" s="14">
+        <v>26</v>
+      </c>
+      <c r="T17" s="14">
+        <v>28</v>
+      </c>
+      <c r="U17" s="14">
+        <v>32</v>
+      </c>
+      <c r="V17" s="14">
+        <v>36</v>
+      </c>
+      <c r="W17" s="14">
+        <v>40</v>
+      </c>
+      <c r="X17" s="14">
+        <v>44</v>
+      </c>
+      <c r="Y17" s="14">
+        <v>48</v>
+      </c>
+      <c r="Z17" s="34">
+        <v>52</v>
+      </c>
+      <c r="AA17" s="34">
+        <v>56</v>
+      </c>
+      <c r="AB17" s="34">
+        <v>60</v>
+      </c>
+      <c r="AC17" s="34">
+        <v>64</v>
+      </c>
+      <c r="AD17" s="34">
+        <v>80</v>
+      </c>
+      <c r="AE17" s="34">
+        <v>96</v>
+      </c>
+      <c r="AF17" s="34">
+        <v>112</v>
+      </c>
+      <c r="AG17" s="34">
+        <v>128</v>
+      </c>
+      <c r="AH17" s="34">
+        <v>144</v>
+      </c>
+      <c r="AI17" s="34">
+        <v>160</v>
+      </c>
+      <c r="AJ17" s="34">
+        <v>176</v>
+      </c>
+      <c r="AK17" s="34">
+        <v>192</v>
+      </c>
+      <c r="AL17" s="3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="3:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="73"/>
+      <c r="F18" s="11">
+        <v>13338</v>
+      </c>
+      <c r="G18" s="17">
+        <v>13326</v>
+      </c>
+      <c r="H18" s="17">
+        <v>13346</v>
+      </c>
+      <c r="I18" s="12">
+        <v>13331</v>
+      </c>
+      <c r="J18" s="12">
+        <v>13337</v>
+      </c>
+      <c r="K18" s="12">
+        <v>13353</v>
+      </c>
+      <c r="L18" s="12">
+        <v>13334</v>
+      </c>
+      <c r="M18" s="12">
+        <v>13356</v>
+      </c>
+      <c r="N18" s="12">
+        <v>13358</v>
+      </c>
+      <c r="O18" s="12">
+        <v>13350</v>
+      </c>
+      <c r="P18" s="12">
+        <v>13348</v>
+      </c>
+      <c r="Q18" s="12">
+        <v>13334</v>
+      </c>
+      <c r="R18" s="12">
+        <v>13336</v>
+      </c>
+      <c r="S18" s="12">
+        <v>13341</v>
+      </c>
+      <c r="T18" s="12">
+        <v>13422</v>
+      </c>
+      <c r="U18" s="12">
+        <v>13360</v>
+      </c>
+      <c r="V18" s="12">
+        <v>13335</v>
+      </c>
+      <c r="W18" s="12">
+        <v>13331</v>
+      </c>
+      <c r="X18" s="12">
+        <v>13328</v>
+      </c>
+      <c r="Y18" s="12">
+        <v>13326</v>
+      </c>
+      <c r="Z18" s="54">
+        <v>13336</v>
+      </c>
+      <c r="AA18" s="54">
+        <v>13332</v>
+      </c>
+      <c r="AB18" s="54">
+        <v>13342</v>
+      </c>
+      <c r="AC18" s="54">
+        <v>13328</v>
+      </c>
+      <c r="AD18" s="54">
+        <v>13425</v>
+      </c>
+      <c r="AE18" s="54">
+        <v>13351</v>
+      </c>
+      <c r="AF18" s="54">
+        <v>13340</v>
+      </c>
+      <c r="AG18" s="54">
+        <v>13329</v>
+      </c>
+      <c r="AH18" s="54">
+        <v>13332</v>
+      </c>
+      <c r="AI18" s="54">
+        <v>13331</v>
+      </c>
+      <c r="AJ18" s="54">
+        <v>13339</v>
+      </c>
+      <c r="AK18" s="54">
+        <v>13338</v>
+      </c>
+      <c r="AL18" s="13">
+        <v>13331</v>
+      </c>
+    </row>
+    <row r="19" spans="3:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="70"/>
+      <c r="D19" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="83"/>
+      <c r="F19" s="4">
+        <v>2407</v>
+      </c>
+      <c r="G19" s="9">
+        <v>2406</v>
+      </c>
+      <c r="H19" s="9">
+        <v>2422</v>
+      </c>
+      <c r="I19" s="1">
+        <v>2406</v>
+      </c>
+      <c r="J19" s="1">
+        <v>2406</v>
+      </c>
+      <c r="K19" s="1">
+        <v>2406</v>
+      </c>
+      <c r="L19" s="1">
+        <v>2407</v>
+      </c>
+      <c r="M19" s="1">
+        <v>2410</v>
+      </c>
+      <c r="N19" s="1">
+        <v>2404</v>
+      </c>
+      <c r="O19" s="1">
+        <v>2406</v>
+      </c>
+      <c r="P19" s="1">
+        <v>2405</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>2405</v>
+      </c>
+      <c r="R19" s="1">
+        <v>2457</v>
+      </c>
+      <c r="S19" s="1">
+        <v>2408</v>
+      </c>
+      <c r="T19" s="1">
+        <v>2400</v>
+      </c>
+      <c r="U19" s="1">
+        <v>2406</v>
+      </c>
+      <c r="V19" s="1">
+        <v>2440</v>
+      </c>
+      <c r="W19" s="1">
+        <v>2405</v>
+      </c>
+      <c r="X19" s="1">
+        <v>2407</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>2407</v>
+      </c>
+      <c r="Z19" s="55">
+        <v>2442</v>
+      </c>
+      <c r="AA19" s="55">
+        <v>2408</v>
+      </c>
+      <c r="AB19" s="55">
+        <v>2408</v>
+      </c>
+      <c r="AC19" s="55">
+        <v>2406</v>
+      </c>
+      <c r="AD19" s="55">
+        <v>2406</v>
+      </c>
+      <c r="AE19" s="55">
+        <v>2406</v>
+      </c>
+      <c r="AF19" s="55">
+        <v>2406</v>
+      </c>
+      <c r="AG19" s="55">
+        <v>2406</v>
+      </c>
+      <c r="AH19" s="55">
+        <v>2398</v>
+      </c>
+      <c r="AI19" s="55">
+        <v>2405</v>
+      </c>
+      <c r="AJ19" s="55">
+        <v>2408</v>
+      </c>
+      <c r="AK19" s="55">
+        <v>2407</v>
+      </c>
+      <c r="AL19" s="5">
+        <v>2408</v>
+      </c>
+    </row>
+    <row r="20" spans="3:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="70"/>
+      <c r="D20" s="72" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="73"/>
+      <c r="F20" s="4">
+        <v>5591</v>
+      </c>
+      <c r="G20" s="9">
+        <v>5593</v>
+      </c>
+      <c r="H20" s="9">
+        <v>5574</v>
+      </c>
+      <c r="I20" s="1">
+        <v>5581</v>
+      </c>
+      <c r="J20" s="1">
+        <v>5573</v>
+      </c>
+      <c r="K20" s="1">
+        <v>5569</v>
+      </c>
+      <c r="L20" s="1">
+        <v>5576</v>
+      </c>
+      <c r="M20" s="1">
+        <v>5571</v>
+      </c>
+      <c r="N20" s="1">
+        <v>5581</v>
+      </c>
+      <c r="O20" s="1">
+        <v>5572</v>
+      </c>
+      <c r="P20" s="1">
+        <v>5576</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>5279</v>
+      </c>
+      <c r="R20" s="1">
+        <v>5592</v>
+      </c>
+      <c r="S20" s="1">
+        <v>5571</v>
+      </c>
+      <c r="T20" s="57">
+        <v>5272</v>
+      </c>
+      <c r="U20" s="1">
+        <v>5572</v>
+      </c>
+      <c r="V20" s="1">
+        <v>5573</v>
+      </c>
+      <c r="W20" s="1">
+        <v>5592</v>
+      </c>
+      <c r="X20" s="1">
+        <v>5589</v>
+      </c>
+      <c r="Y20" s="1">
+        <v>5574</v>
+      </c>
+      <c r="Z20" s="55">
+        <v>5572</v>
+      </c>
+      <c r="AA20" s="55">
+        <v>5576</v>
+      </c>
+      <c r="AB20" s="55">
+        <v>5575</v>
+      </c>
+      <c r="AC20" s="55">
+        <v>5572</v>
+      </c>
+      <c r="AD20" s="55">
+        <v>5574</v>
+      </c>
+      <c r="AE20" s="55">
+        <v>5571</v>
+      </c>
+      <c r="AF20" s="55">
+        <v>5571</v>
+      </c>
+      <c r="AG20" s="55">
+        <v>5575</v>
+      </c>
+      <c r="AH20" s="55">
+        <v>5591</v>
+      </c>
+      <c r="AI20" s="55">
+        <v>5574</v>
+      </c>
+      <c r="AJ20" s="55">
+        <v>5575</v>
+      </c>
+      <c r="AK20" s="55">
+        <v>5572</v>
+      </c>
+      <c r="AL20" s="5">
+        <v>5590</v>
+      </c>
+    </row>
+    <row r="21" spans="3:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="71"/>
+      <c r="D21" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="75"/>
+      <c r="F21" s="6">
+        <v>295270</v>
+      </c>
+      <c r="G21" s="10">
+        <v>295490</v>
+      </c>
+      <c r="H21" s="10">
+        <v>295292</v>
+      </c>
+      <c r="I21" s="7">
+        <v>295395</v>
+      </c>
+      <c r="J21" s="7">
+        <v>295319</v>
+      </c>
+      <c r="K21" s="7">
+        <v>295301</v>
+      </c>
+      <c r="L21" s="7">
+        <v>295425</v>
+      </c>
+      <c r="M21" s="7">
+        <v>295290</v>
+      </c>
+      <c r="N21" s="7">
+        <v>295767</v>
+      </c>
+      <c r="O21" s="7">
+        <v>295320</v>
+      </c>
+      <c r="P21" s="7">
+        <v>295443</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>295273</v>
+      </c>
+      <c r="R21" s="7">
+        <v>295390</v>
+      </c>
+      <c r="S21" s="7">
+        <v>296454</v>
+      </c>
+      <c r="T21" s="7">
+        <v>295271</v>
+      </c>
+      <c r="U21" s="7">
+        <v>295477</v>
+      </c>
+      <c r="V21" s="7">
+        <v>295445</v>
+      </c>
+      <c r="W21" s="7">
+        <v>295287</v>
+      </c>
+      <c r="X21" s="7">
+        <v>295262</v>
+      </c>
+      <c r="Y21" s="7">
+        <v>295274</v>
+      </c>
+      <c r="Z21" s="56">
+        <v>295325</v>
+      </c>
+      <c r="AA21" s="56">
+        <v>295305</v>
+      </c>
+      <c r="AB21" s="56">
+        <v>295270</v>
+      </c>
+      <c r="AC21" s="56">
+        <v>295394</v>
+      </c>
+      <c r="AD21" s="56">
+        <v>295293</v>
+      </c>
+      <c r="AE21" s="56">
+        <v>297213</v>
+      </c>
+      <c r="AF21" s="56">
+        <v>295498</v>
+      </c>
+      <c r="AG21" s="56">
+        <v>295272</v>
+      </c>
+      <c r="AH21" s="56">
+        <v>295274</v>
+      </c>
+      <c r="AI21" s="56">
+        <v>295269</v>
+      </c>
+      <c r="AJ21" s="56">
+        <v>295512</v>
+      </c>
+      <c r="AK21" s="56">
+        <v>295312</v>
+      </c>
+      <c r="AL21" s="8">
+        <v>295719</v>
+      </c>
+    </row>
+    <row r="22" spans="3:38" x14ac:dyDescent="0.25">
+      <c r="F22" s="101" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="102"/>
+      <c r="H22" s="102"/>
+      <c r="I22" s="102"/>
+      <c r="J22" s="102"/>
+      <c r="K22" s="102"/>
+      <c r="L22" s="102"/>
+      <c r="M22" s="102"/>
+      <c r="N22" s="102"/>
+      <c r="O22" s="102"/>
+      <c r="P22" s="102"/>
+      <c r="Q22" s="102"/>
+      <c r="R22" s="102"/>
+      <c r="S22" s="102"/>
+      <c r="T22" s="102"/>
+      <c r="U22" s="102"/>
+      <c r="V22" s="102"/>
+      <c r="W22" s="102"/>
+      <c r="X22" s="102"/>
+      <c r="Y22" s="102"/>
+      <c r="Z22" s="102"/>
+      <c r="AA22" s="102"/>
+      <c r="AB22" s="102"/>
+      <c r="AC22" s="102"/>
+      <c r="AD22" s="102"/>
+      <c r="AE22" s="102"/>
+      <c r="AF22" s="102"/>
+      <c r="AG22" s="102"/>
+      <c r="AH22" s="102"/>
+      <c r="AI22" s="102"/>
+      <c r="AJ22" s="102"/>
+      <c r="AK22" s="102"/>
+      <c r="AL22" s="103"/>
+    </row>
+    <row r="23" spans="3:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="104"/>
+      <c r="G23" s="105"/>
+      <c r="H23" s="105"/>
+      <c r="I23" s="105"/>
+      <c r="J23" s="105"/>
+      <c r="K23" s="105"/>
+      <c r="L23" s="105"/>
+      <c r="M23" s="105"/>
+      <c r="N23" s="105"/>
+      <c r="O23" s="105"/>
+      <c r="P23" s="105"/>
+      <c r="Q23" s="105"/>
+      <c r="R23" s="105"/>
+      <c r="S23" s="105"/>
+      <c r="T23" s="105"/>
+      <c r="U23" s="105"/>
+      <c r="V23" s="105"/>
+      <c r="W23" s="105"/>
+      <c r="X23" s="105"/>
+      <c r="Y23" s="105"/>
+      <c r="Z23" s="105"/>
+      <c r="AA23" s="105"/>
+      <c r="AB23" s="105"/>
+      <c r="AC23" s="105"/>
+      <c r="AD23" s="105"/>
+      <c r="AE23" s="105"/>
+      <c r="AF23" s="105"/>
+      <c r="AG23" s="105"/>
+      <c r="AH23" s="105"/>
+      <c r="AI23" s="105"/>
+      <c r="AJ23" s="105"/>
+      <c r="AK23" s="105"/>
+      <c r="AL23" s="106"/>
+    </row>
+    <row r="24" spans="3:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="80" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="81"/>
+      <c r="F24" s="2">
+        <v>1</v>
+      </c>
+      <c r="G24" s="16">
+        <v>2</v>
+      </c>
+      <c r="H24" s="16">
+        <v>4</v>
+      </c>
+      <c r="I24" s="14">
+        <v>6</v>
+      </c>
+      <c r="J24" s="14">
+        <v>8</v>
+      </c>
+      <c r="K24" s="14">
+        <v>10</v>
+      </c>
+      <c r="L24" s="14">
+        <v>12</v>
+      </c>
+      <c r="M24" s="14">
+        <v>14</v>
+      </c>
+      <c r="N24" s="14">
+        <v>16</v>
+      </c>
+      <c r="O24" s="14">
+        <v>18</v>
+      </c>
+      <c r="P24" s="14">
+        <v>20</v>
+      </c>
+      <c r="Q24" s="14">
+        <v>22</v>
+      </c>
+      <c r="R24" s="14">
+        <v>24</v>
+      </c>
+      <c r="S24" s="14">
+        <v>26</v>
+      </c>
+      <c r="T24" s="14">
+        <v>28</v>
+      </c>
+      <c r="U24" s="14">
+        <v>32</v>
+      </c>
+      <c r="V24" s="14">
+        <v>36</v>
+      </c>
+      <c r="W24" s="14">
+        <v>40</v>
+      </c>
+      <c r="X24" s="14">
+        <v>44</v>
+      </c>
+      <c r="Y24" s="14">
+        <v>48</v>
+      </c>
+      <c r="Z24" s="34">
+        <v>52</v>
+      </c>
+      <c r="AA24" s="34">
+        <v>56</v>
+      </c>
+      <c r="AB24" s="34">
+        <v>60</v>
+      </c>
+      <c r="AC24" s="34">
+        <v>64</v>
+      </c>
+      <c r="AD24" s="34">
+        <v>80</v>
+      </c>
+      <c r="AE24" s="34">
+        <v>96</v>
+      </c>
+      <c r="AF24" s="34">
+        <v>112</v>
+      </c>
+      <c r="AG24" s="34">
+        <v>128</v>
+      </c>
+      <c r="AH24" s="34">
+        <v>144</v>
+      </c>
+      <c r="AI24" s="34">
+        <v>160</v>
+      </c>
+      <c r="AJ24" s="34">
+        <v>176</v>
+      </c>
+      <c r="AK24" s="34">
+        <v>192</v>
+      </c>
+      <c r="AL24" s="3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="3:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="73"/>
+      <c r="F25" s="11">
+        <v>9549</v>
+      </c>
+      <c r="G25" s="17">
+        <v>9565</v>
+      </c>
+      <c r="H25" s="17">
+        <v>9568</v>
+      </c>
+      <c r="I25" s="12">
+        <v>9578</v>
+      </c>
+      <c r="J25" s="12">
+        <v>9578</v>
+      </c>
+      <c r="K25" s="12">
+        <v>9581</v>
+      </c>
+      <c r="L25" s="12">
+        <v>9577</v>
+      </c>
+      <c r="M25" s="12">
+        <v>9586</v>
+      </c>
+      <c r="N25" s="12">
+        <v>9587</v>
+      </c>
+      <c r="O25" s="12">
+        <v>9573</v>
+      </c>
+      <c r="P25" s="12">
+        <v>9610</v>
+      </c>
+      <c r="Q25" s="12">
+        <v>9577</v>
+      </c>
+      <c r="R25" s="12">
+        <v>9632</v>
+      </c>
+      <c r="S25" s="12">
+        <v>9617</v>
+      </c>
+      <c r="T25" s="12">
+        <v>9592</v>
+      </c>
+      <c r="U25" s="12">
+        <v>9601</v>
+      </c>
+      <c r="V25" s="12">
+        <v>9630</v>
+      </c>
+      <c r="W25" s="12">
+        <v>9717</v>
+      </c>
+      <c r="X25" s="12">
+        <v>9660</v>
+      </c>
+      <c r="Y25" s="12">
+        <v>9742</v>
+      </c>
+      <c r="Z25" s="54">
+        <v>9627</v>
+      </c>
+      <c r="AA25" s="54">
+        <v>9652</v>
+      </c>
+      <c r="AB25" s="54">
+        <v>9679</v>
+      </c>
+      <c r="AC25" s="54">
+        <v>9591</v>
+      </c>
+      <c r="AD25" s="54">
+        <v>10000</v>
+      </c>
+      <c r="AE25" s="54">
+        <v>9936</v>
+      </c>
+      <c r="AF25" s="54">
+        <v>10006</v>
+      </c>
+      <c r="AG25" s="54">
+        <v>10008</v>
+      </c>
+      <c r="AH25" s="54">
+        <v>10147</v>
+      </c>
+      <c r="AI25" s="54">
+        <v>10320</v>
+      </c>
+      <c r="AJ25" s="54">
+        <v>9944</v>
+      </c>
+      <c r="AK25" s="54">
+        <v>10113</v>
+      </c>
+      <c r="AL25" s="13">
+        <v>10590</v>
+      </c>
+    </row>
+    <row r="26" spans="3:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="70"/>
+      <c r="D26" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="83"/>
+      <c r="F26" s="4">
+        <v>1589</v>
+      </c>
+      <c r="G26" s="9">
+        <v>1590</v>
+      </c>
+      <c r="H26" s="9">
+        <v>1591</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1589</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1587</v>
+      </c>
+      <c r="K26" s="1">
+        <v>1588</v>
+      </c>
+      <c r="L26" s="1">
+        <v>1597</v>
+      </c>
+      <c r="M26" s="1">
+        <v>1593</v>
+      </c>
+      <c r="N26" s="1">
+        <v>1648</v>
+      </c>
+      <c r="O26" s="1">
+        <v>1591</v>
+      </c>
+      <c r="P26" s="1">
+        <v>1597</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>1597</v>
+      </c>
+      <c r="R26" s="1">
+        <v>1603</v>
+      </c>
+      <c r="S26" s="1">
+        <v>1602</v>
+      </c>
+      <c r="T26" s="1">
+        <v>1593</v>
+      </c>
+      <c r="U26" s="1">
+        <v>1599</v>
+      </c>
+      <c r="V26" s="1">
+        <v>1616</v>
+      </c>
+      <c r="W26" s="1">
+        <v>1591</v>
+      </c>
+      <c r="X26" s="1">
+        <v>1623</v>
+      </c>
+      <c r="Y26" s="1">
+        <v>1615</v>
+      </c>
+      <c r="Z26" s="55">
+        <v>1603</v>
+      </c>
+      <c r="AA26" s="55">
+        <v>1612</v>
+      </c>
+      <c r="AB26" s="55">
+        <v>1601</v>
+      </c>
+      <c r="AC26" s="55">
+        <v>1624</v>
+      </c>
+      <c r="AD26" s="55">
+        <v>1605</v>
+      </c>
+      <c r="AE26" s="55">
+        <v>1591</v>
+      </c>
+      <c r="AF26" s="55">
+        <v>1687</v>
+      </c>
+      <c r="AG26" s="55">
+        <v>1823</v>
+      </c>
+      <c r="AH26" s="55">
+        <v>1784</v>
+      </c>
+      <c r="AI26" s="55">
+        <v>1953</v>
+      </c>
+      <c r="AJ26" s="55">
+        <v>1895</v>
+      </c>
+      <c r="AK26" s="55">
+        <v>1679</v>
+      </c>
+      <c r="AL26" s="5">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="27" spans="3:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="70"/>
+      <c r="D27" s="72" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="73"/>
+      <c r="F27" s="4">
+        <v>2800</v>
+      </c>
+      <c r="G27" s="9">
+        <v>2800</v>
+      </c>
+      <c r="H27" s="9">
+        <v>2818</v>
+      </c>
+      <c r="I27" s="1">
+        <v>2808</v>
+      </c>
+      <c r="J27" s="1">
+        <v>2805</v>
+      </c>
+      <c r="K27" s="1">
+        <v>2800</v>
+      </c>
+      <c r="L27" s="1">
+        <v>2805</v>
+      </c>
+      <c r="M27" s="1">
+        <v>2807</v>
+      </c>
+      <c r="N27" s="1">
+        <v>2805</v>
+      </c>
+      <c r="O27" s="1">
+        <v>2859</v>
+      </c>
+      <c r="P27" s="1">
+        <v>2798</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>2821</v>
+      </c>
+      <c r="R27" s="1">
+        <v>2826</v>
+      </c>
+      <c r="S27" s="1">
+        <v>2814</v>
+      </c>
+      <c r="T27" s="1">
+        <v>2849</v>
+      </c>
+      <c r="U27" s="1">
+        <v>2834</v>
+      </c>
+      <c r="V27" s="1">
+        <v>2829</v>
+      </c>
+      <c r="W27" s="1">
+        <v>2816</v>
+      </c>
+      <c r="X27" s="1">
+        <v>2821</v>
+      </c>
+      <c r="Y27" s="1">
+        <v>2864</v>
+      </c>
+      <c r="Z27" s="55">
+        <v>2891</v>
+      </c>
+      <c r="AA27" s="55">
+        <v>2870</v>
+      </c>
+      <c r="AB27" s="55">
+        <v>2960</v>
+      </c>
+      <c r="AC27" s="55">
+        <v>2955</v>
+      </c>
+      <c r="AD27" s="55">
+        <v>3045</v>
+      </c>
+      <c r="AE27" s="55">
+        <v>3267</v>
+      </c>
+      <c r="AF27" s="55">
+        <v>3351</v>
+      </c>
+      <c r="AG27" s="55">
+        <v>3484</v>
+      </c>
+      <c r="AH27" s="55">
+        <v>3506</v>
+      </c>
+      <c r="AI27" s="55">
+        <v>3941</v>
+      </c>
+      <c r="AJ27" s="55">
+        <v>3837</v>
+      </c>
+      <c r="AK27" s="55">
+        <v>4119</v>
+      </c>
+      <c r="AL27" s="5">
+        <v>4369</v>
+      </c>
+    </row>
+    <row r="28" spans="3:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="71"/>
+      <c r="D28" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="75"/>
+      <c r="F28" s="6">
+        <v>250708</v>
+      </c>
+      <c r="G28" s="10">
+        <v>250590</v>
+      </c>
+      <c r="H28" s="10">
+        <v>250502</v>
+      </c>
+      <c r="I28" s="7">
+        <v>250725</v>
+      </c>
+      <c r="J28" s="7">
+        <v>251646</v>
+      </c>
+      <c r="K28" s="7">
+        <v>252398</v>
+      </c>
+      <c r="L28" s="7">
+        <v>250845</v>
+      </c>
+      <c r="M28" s="7">
+        <v>251079</v>
+      </c>
+      <c r="N28" s="7">
+        <v>250771</v>
+      </c>
+      <c r="O28" s="7">
+        <v>250632</v>
+      </c>
+      <c r="P28" s="7">
+        <v>250503</v>
+      </c>
+      <c r="Q28" s="7">
+        <v>251749</v>
+      </c>
+      <c r="R28" s="7">
+        <v>250929</v>
+      </c>
+      <c r="S28" s="7">
+        <v>252228</v>
+      </c>
+      <c r="T28" s="7">
+        <v>251206</v>
+      </c>
+      <c r="U28" s="7">
+        <v>250634</v>
+      </c>
+      <c r="V28" s="7">
+        <v>251185</v>
+      </c>
+      <c r="W28" s="7">
+        <v>251275</v>
+      </c>
+      <c r="X28" s="7">
+        <v>250934</v>
+      </c>
+      <c r="Y28" s="7">
+        <v>251518</v>
+      </c>
+      <c r="Z28" s="56">
+        <v>253448</v>
+      </c>
+      <c r="AA28" s="56">
+        <v>256264</v>
+      </c>
+      <c r="AB28" s="56">
+        <v>253440</v>
+      </c>
+      <c r="AC28" s="56">
+        <v>253291</v>
+      </c>
+      <c r="AD28" s="56">
+        <v>251583</v>
+      </c>
+      <c r="AE28" s="56">
+        <v>252719</v>
+      </c>
+      <c r="AF28" s="56">
+        <v>256021</v>
+      </c>
+      <c r="AG28" s="56">
+        <v>253549</v>
+      </c>
+      <c r="AH28" s="56">
+        <v>253365</v>
+      </c>
+      <c r="AI28" s="56">
+        <v>252090</v>
+      </c>
+      <c r="AJ28" s="56">
+        <v>252709</v>
+      </c>
+      <c r="AK28" s="56">
+        <v>256371</v>
+      </c>
+      <c r="AL28" s="8">
+        <v>256287</v>
+      </c>
+    </row>
+    <row r="29" spans="3:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="3:38" x14ac:dyDescent="0.25">
+      <c r="F30" s="109" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="110"/>
+    </row>
+    <row r="31" spans="3:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F31" s="111"/>
+      <c r="G31" s="112"/>
+    </row>
+    <row r="32" spans="3:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="86"/>
+      <c r="F32" s="113">
+        <v>25714</v>
+      </c>
+      <c r="G32" s="114"/>
+    </row>
+    <row r="33" spans="3:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="70"/>
+      <c r="D33" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="87"/>
+      <c r="F33" s="115">
+        <v>3999</v>
+      </c>
+      <c r="G33" s="116"/>
+    </row>
+    <row r="34" spans="3:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="70"/>
+      <c r="D34" s="72" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="86"/>
+      <c r="F34" s="115">
+        <v>6628</v>
+      </c>
+      <c r="G34" s="116"/>
+    </row>
+    <row r="35" spans="3:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="71"/>
+      <c r="D35" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" s="88"/>
+      <c r="F35" s="107">
+        <v>843395</v>
+      </c>
+      <c r="G35" s="108"/>
+    </row>
+    <row r="39" spans="3:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="3:53" x14ac:dyDescent="0.25">
+      <c r="F40" s="117" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" s="118"/>
+      <c r="H40" s="118"/>
+      <c r="I40" s="118"/>
+      <c r="J40" s="118"/>
+      <c r="K40" s="118"/>
+      <c r="L40" s="118"/>
+      <c r="M40" s="118"/>
+      <c r="N40" s="118"/>
+      <c r="O40" s="118"/>
+      <c r="P40" s="118"/>
+      <c r="Q40" s="118"/>
+      <c r="R40" s="118"/>
+      <c r="S40" s="118"/>
+      <c r="T40" s="118"/>
+      <c r="U40" s="118"/>
+      <c r="V40" s="118"/>
+      <c r="W40" s="118"/>
+      <c r="X40" s="118"/>
+      <c r="Y40" s="118"/>
+      <c r="Z40" s="118"/>
+      <c r="AA40" s="118"/>
+      <c r="AB40" s="118"/>
+      <c r="AC40" s="118"/>
+      <c r="AD40" s="118"/>
+      <c r="AE40" s="118"/>
+      <c r="AF40" s="118"/>
+      <c r="AG40" s="118"/>
+      <c r="AH40" s="118"/>
+      <c r="AI40" s="118"/>
+      <c r="AJ40" s="118"/>
+      <c r="AK40" s="118"/>
+      <c r="AL40" s="118"/>
+      <c r="AM40" s="118"/>
+      <c r="AN40" s="118"/>
+      <c r="AO40" s="118"/>
+      <c r="AP40" s="118"/>
+      <c r="AQ40" s="118"/>
+      <c r="AR40" s="118"/>
+      <c r="AS40" s="118"/>
+      <c r="AT40" s="118"/>
+      <c r="AU40" s="118"/>
+      <c r="AV40" s="118"/>
+      <c r="AW40" s="118"/>
+      <c r="AX40" s="118"/>
+      <c r="AY40" s="118"/>
+      <c r="AZ40" s="118"/>
+      <c r="BA40" s="119"/>
+    </row>
+    <row r="41" spans="3:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F41" s="120"/>
+      <c r="G41" s="121"/>
+      <c r="H41" s="121"/>
+      <c r="I41" s="121"/>
+      <c r="J41" s="121"/>
+      <c r="K41" s="121"/>
+      <c r="L41" s="121"/>
+      <c r="M41" s="121"/>
+      <c r="N41" s="121"/>
+      <c r="O41" s="121"/>
+      <c r="P41" s="121"/>
+      <c r="Q41" s="121"/>
+      <c r="R41" s="121"/>
+      <c r="S41" s="121"/>
+      <c r="T41" s="121"/>
+      <c r="U41" s="121"/>
+      <c r="V41" s="121"/>
+      <c r="W41" s="121"/>
+      <c r="X41" s="121"/>
+      <c r="Y41" s="121"/>
+      <c r="Z41" s="121"/>
+      <c r="AA41" s="121"/>
+      <c r="AB41" s="121"/>
+      <c r="AC41" s="121"/>
+      <c r="AD41" s="121"/>
+      <c r="AE41" s="121"/>
+      <c r="AF41" s="121"/>
+      <c r="AG41" s="121"/>
+      <c r="AH41" s="121"/>
+      <c r="AI41" s="121"/>
+      <c r="AJ41" s="121"/>
+      <c r="AK41" s="121"/>
+      <c r="AL41" s="121"/>
+      <c r="AM41" s="121"/>
+      <c r="AN41" s="121"/>
+      <c r="AO41" s="121"/>
+      <c r="AP41" s="121"/>
+      <c r="AQ41" s="121"/>
+      <c r="AR41" s="121"/>
+      <c r="AS41" s="121"/>
+      <c r="AT41" s="121"/>
+      <c r="AU41" s="121"/>
+      <c r="AV41" s="121"/>
+      <c r="AW41" s="121"/>
+      <c r="AX41" s="121"/>
+      <c r="AY41" s="121"/>
+      <c r="AZ41" s="121"/>
+      <c r="BA41" s="122"/>
+    </row>
+    <row r="42" spans="3:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D42" s="80" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="85"/>
+      <c r="F42" s="2">
+        <v>1</v>
+      </c>
+      <c r="G42" s="14">
+        <v>2</v>
+      </c>
+      <c r="H42" s="14">
+        <v>4</v>
+      </c>
+      <c r="I42" s="14">
+        <v>6</v>
+      </c>
+      <c r="J42" s="14">
+        <v>8</v>
+      </c>
+      <c r="K42" s="14">
+        <v>10</v>
+      </c>
+      <c r="L42" s="14">
+        <v>12</v>
+      </c>
+      <c r="M42" s="14">
+        <v>14</v>
+      </c>
+      <c r="N42" s="14">
+        <v>16</v>
+      </c>
+      <c r="O42" s="14">
+        <v>18</v>
+      </c>
+      <c r="P42" s="14">
+        <v>20</v>
+      </c>
+      <c r="Q42" s="14">
+        <v>22</v>
+      </c>
+      <c r="R42" s="14">
+        <v>24</v>
+      </c>
+      <c r="S42" s="14">
+        <v>26</v>
+      </c>
+      <c r="T42" s="14">
+        <v>28</v>
+      </c>
+      <c r="U42" s="14">
+        <v>32</v>
+      </c>
+      <c r="V42" s="14">
+        <v>36</v>
+      </c>
+      <c r="W42" s="14">
+        <v>40</v>
+      </c>
+      <c r="X42" s="14">
+        <v>44</v>
+      </c>
+      <c r="Y42" s="14">
+        <v>48</v>
+      </c>
+      <c r="Z42" s="14">
+        <v>52</v>
+      </c>
+      <c r="AA42" s="14">
+        <v>56</v>
+      </c>
+      <c r="AB42" s="14">
+        <v>60</v>
+      </c>
+      <c r="AC42" s="14">
+        <v>64</v>
+      </c>
+      <c r="AD42" s="14">
+        <v>80</v>
+      </c>
+      <c r="AE42" s="14">
+        <v>96</v>
+      </c>
+      <c r="AF42" s="14">
+        <v>112</v>
+      </c>
+      <c r="AG42" s="14">
+        <v>128</v>
+      </c>
+      <c r="AH42" s="14">
+        <v>144</v>
+      </c>
+      <c r="AI42" s="14">
+        <v>160</v>
+      </c>
+      <c r="AJ42" s="14">
+        <v>176</v>
+      </c>
+      <c r="AK42" s="14">
+        <v>192</v>
+      </c>
+      <c r="AL42" s="14">
+        <v>208</v>
+      </c>
+      <c r="AM42" s="14">
+        <v>224</v>
+      </c>
+      <c r="AN42" s="14">
+        <v>240</v>
+      </c>
+      <c r="AO42" s="14">
+        <v>256</v>
+      </c>
+      <c r="AP42" s="14">
+        <v>272</v>
+      </c>
+      <c r="AQ42" s="14">
+        <v>288</v>
+      </c>
+      <c r="AR42" s="14">
+        <v>304</v>
+      </c>
+      <c r="AS42" s="14">
+        <v>320</v>
+      </c>
+      <c r="AT42" s="14">
+        <v>336</v>
+      </c>
+      <c r="AU42" s="14">
+        <v>352</v>
+      </c>
+      <c r="AV42" s="14">
+        <v>368</v>
+      </c>
+      <c r="AW42" s="14">
+        <v>384</v>
+      </c>
+      <c r="AX42" s="14">
+        <v>400</v>
+      </c>
+      <c r="AY42" s="14">
+        <v>416</v>
+      </c>
+      <c r="AZ42" s="14">
+        <v>432</v>
+      </c>
+      <c r="BA42" s="3">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="43" spans="3:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="86"/>
+      <c r="F43" s="11">
+        <v>38113</v>
+      </c>
+      <c r="G43" s="12">
+        <v>19089</v>
+      </c>
+      <c r="H43" s="12">
+        <v>9564</v>
+      </c>
+      <c r="I43" s="12">
+        <v>6385</v>
+      </c>
+      <c r="J43" s="12">
+        <v>4804</v>
+      </c>
+      <c r="K43" s="12">
+        <v>3848</v>
+      </c>
+      <c r="L43" s="12">
+        <v>3214</v>
+      </c>
+      <c r="M43" s="12">
+        <v>2763</v>
+      </c>
+      <c r="N43" s="12">
+        <v>2425</v>
+      </c>
+      <c r="O43" s="12">
+        <v>2160</v>
+      </c>
+      <c r="P43" s="12">
+        <v>1951</v>
+      </c>
+      <c r="Q43" s="12">
+        <v>1776</v>
+      </c>
+      <c r="R43" s="12">
+        <v>1633</v>
+      </c>
+      <c r="S43" s="12">
+        <v>1526</v>
+      </c>
+      <c r="T43" s="12">
+        <v>1407</v>
+      </c>
+      <c r="U43" s="12">
+        <v>1251</v>
+      </c>
+      <c r="V43" s="12">
+        <v>1118</v>
+      </c>
+      <c r="W43" s="12">
+        <v>1001</v>
+      </c>
+      <c r="X43" s="12">
+        <v>918</v>
+      </c>
+      <c r="Y43" s="12">
+        <v>877</v>
+      </c>
+      <c r="Z43" s="12">
+        <v>837</v>
+      </c>
+      <c r="AA43" s="12">
+        <v>775</v>
+      </c>
+      <c r="AB43" s="12">
+        <v>722</v>
+      </c>
+      <c r="AC43" s="12">
+        <v>724</v>
+      </c>
+      <c r="AD43" s="12">
+        <v>633</v>
+      </c>
+      <c r="AE43" s="12">
+        <v>561</v>
+      </c>
+      <c r="AF43" s="12">
+        <v>526</v>
+      </c>
+      <c r="AG43" s="12">
+        <v>490</v>
+      </c>
+      <c r="AH43" s="12">
+        <v>466</v>
+      </c>
+      <c r="AI43" s="12">
+        <v>445</v>
+      </c>
+      <c r="AJ43" s="12">
+        <v>426</v>
+      </c>
+      <c r="AK43" s="12">
+        <v>404</v>
+      </c>
+      <c r="AL43" s="12">
+        <v>400</v>
+      </c>
+      <c r="AM43" s="124">
+        <v>397</v>
+      </c>
+      <c r="AN43" s="124">
+        <v>399</v>
+      </c>
+      <c r="AO43" s="124">
+        <v>401</v>
+      </c>
+      <c r="AP43" s="124">
+        <v>404</v>
+      </c>
+      <c r="AQ43" s="124">
+        <v>403</v>
+      </c>
+      <c r="AR43" s="124">
+        <v>404</v>
+      </c>
+      <c r="AS43" s="124">
+        <v>403</v>
+      </c>
+      <c r="AT43" s="124">
+        <v>409</v>
+      </c>
+      <c r="AU43" s="124">
+        <v>404</v>
+      </c>
+      <c r="AV43" s="124">
+        <v>408</v>
+      </c>
+      <c r="AW43" s="124">
+        <v>407</v>
+      </c>
+      <c r="AX43" s="124">
+        <v>404</v>
+      </c>
+      <c r="AY43" s="124">
+        <v>409</v>
+      </c>
+      <c r="AZ43" s="124">
+        <v>413</v>
+      </c>
+      <c r="BA43" s="125">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="44" spans="3:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="70"/>
+      <c r="D44" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="87"/>
+      <c r="F44" s="4">
+        <v>6197</v>
+      </c>
+      <c r="G44" s="1">
+        <v>3128</v>
+      </c>
+      <c r="H44" s="1">
+        <v>1595</v>
+      </c>
+      <c r="I44" s="1">
+        <v>1068</v>
+      </c>
+      <c r="J44" s="1">
+        <v>814</v>
+      </c>
+      <c r="K44" s="1">
+        <v>664</v>
+      </c>
+      <c r="L44" s="1">
+        <v>557</v>
+      </c>
+      <c r="M44" s="1">
+        <v>483</v>
+      </c>
+      <c r="N44" s="1">
+        <v>428</v>
+      </c>
+      <c r="O44" s="1">
+        <v>391</v>
+      </c>
+      <c r="P44" s="1">
+        <v>353</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>325</v>
+      </c>
+      <c r="R44" s="1">
+        <v>301</v>
+      </c>
+      <c r="S44" s="1">
+        <v>282</v>
+      </c>
+      <c r="T44" s="1">
+        <v>265</v>
+      </c>
+      <c r="U44" s="1">
+        <v>236</v>
+      </c>
+      <c r="V44" s="1">
+        <v>216</v>
+      </c>
+      <c r="W44" s="1">
+        <v>199</v>
+      </c>
+      <c r="X44" s="1">
+        <v>184</v>
+      </c>
+      <c r="Y44" s="1">
+        <v>177</v>
+      </c>
+      <c r="Z44" s="1">
+        <v>167</v>
+      </c>
+      <c r="AA44" s="1">
+        <v>159</v>
+      </c>
+      <c r="AB44" s="1">
+        <v>152</v>
+      </c>
+      <c r="AC44" s="1">
+        <v>146</v>
+      </c>
+      <c r="AD44" s="1">
+        <v>129</v>
+      </c>
+      <c r="AE44" s="1">
+        <v>114</v>
+      </c>
+      <c r="AF44" s="1">
+        <v>131</v>
+      </c>
+      <c r="AG44" s="1">
+        <v>134</v>
+      </c>
+      <c r="AH44" s="1">
+        <v>128</v>
+      </c>
+      <c r="AI44" s="1">
+        <v>128</v>
+      </c>
+      <c r="AJ44" s="1">
+        <v>132</v>
+      </c>
+      <c r="AK44" s="1">
+        <v>132</v>
+      </c>
+      <c r="AL44" s="1">
+        <v>133</v>
+      </c>
+      <c r="AM44" s="123">
+        <v>137</v>
+      </c>
+      <c r="AN44" s="123">
+        <v>135</v>
+      </c>
+      <c r="AO44" s="123">
+        <v>135</v>
+      </c>
+      <c r="AP44" s="123">
+        <v>129</v>
+      </c>
+      <c r="AQ44" s="123">
+        <v>131</v>
+      </c>
+      <c r="AR44" s="123">
+        <v>137</v>
+      </c>
+      <c r="AS44" s="123">
+        <v>130</v>
+      </c>
+      <c r="AT44" s="123">
+        <v>135</v>
+      </c>
+      <c r="AU44" s="123">
+        <v>131</v>
+      </c>
+      <c r="AV44" s="123">
+        <v>128</v>
+      </c>
+      <c r="AW44" s="123">
+        <v>134</v>
+      </c>
+      <c r="AX44" s="123">
+        <v>132</v>
+      </c>
+      <c r="AY44" s="123">
+        <v>131</v>
+      </c>
+      <c r="AZ44" s="123">
+        <v>132</v>
+      </c>
+      <c r="BA44" s="126">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="3:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="70"/>
+      <c r="D45" s="72" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="86"/>
+      <c r="F45" s="4">
+        <v>11039</v>
+      </c>
+      <c r="G45" s="1">
+        <v>5531</v>
+      </c>
+      <c r="H45" s="1">
+        <v>2797</v>
+      </c>
+      <c r="I45" s="1">
+        <v>1883</v>
+      </c>
+      <c r="J45" s="1">
+        <v>1421</v>
+      </c>
+      <c r="K45" s="1">
+        <v>1142</v>
+      </c>
+      <c r="L45" s="1">
+        <v>957</v>
+      </c>
+      <c r="M45" s="1">
+        <v>827</v>
+      </c>
+      <c r="N45" s="1">
+        <v>729</v>
+      </c>
+      <c r="O45" s="1">
+        <v>654</v>
+      </c>
+      <c r="P45" s="1">
+        <v>594</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>545</v>
+      </c>
+      <c r="R45" s="1">
+        <v>503</v>
+      </c>
+      <c r="S45" s="1">
+        <v>468</v>
+      </c>
+      <c r="T45" s="1">
+        <v>438</v>
+      </c>
+      <c r="U45" s="1">
+        <v>389</v>
+      </c>
+      <c r="V45" s="1">
+        <v>352</v>
+      </c>
+      <c r="W45" s="1">
+        <v>322</v>
+      </c>
+      <c r="X45" s="1">
+        <v>299</v>
+      </c>
+      <c r="Y45" s="1">
+        <v>281</v>
+      </c>
+      <c r="Z45" s="1">
+        <v>272</v>
+      </c>
+      <c r="AA45" s="1">
+        <v>259</v>
+      </c>
+      <c r="AB45" s="1">
+        <v>239</v>
+      </c>
+      <c r="AC45" s="1">
+        <v>235</v>
+      </c>
+      <c r="AD45" s="1">
+        <v>216</v>
+      </c>
+      <c r="AE45" s="1">
+        <v>228</v>
+      </c>
+      <c r="AF45" s="1">
+        <v>232</v>
+      </c>
+      <c r="AG45" s="1">
+        <v>226</v>
+      </c>
+      <c r="AH45" s="1">
+        <v>227</v>
+      </c>
+      <c r="AI45" s="1">
+        <v>223</v>
+      </c>
+      <c r="AJ45" s="1">
+        <v>227</v>
+      </c>
+      <c r="AK45" s="1">
+        <v>233</v>
+      </c>
+      <c r="AL45" s="1">
+        <v>235</v>
+      </c>
+      <c r="AM45" s="123">
+        <v>222</v>
+      </c>
+      <c r="AN45" s="123">
+        <v>230</v>
+      </c>
+      <c r="AO45" s="123">
+        <v>222</v>
+      </c>
+      <c r="AP45" s="123">
+        <v>222</v>
+      </c>
+      <c r="AQ45" s="123">
+        <v>214</v>
+      </c>
+      <c r="AR45" s="123">
+        <v>233</v>
+      </c>
+      <c r="AS45" s="123">
+        <v>229</v>
+      </c>
+      <c r="AT45" s="123">
+        <v>218</v>
+      </c>
+      <c r="AU45" s="123">
+        <v>215</v>
+      </c>
+      <c r="AV45" s="123">
+        <v>218</v>
+      </c>
+      <c r="AW45" s="123">
+        <v>225</v>
+      </c>
+      <c r="AX45" s="123">
+        <v>230</v>
+      </c>
+      <c r="AY45" s="123">
+        <v>231</v>
+      </c>
+      <c r="AZ45" s="123">
+        <v>233</v>
+      </c>
+      <c r="BA45" s="126">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="46" spans="3:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="71"/>
+      <c r="D46" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46" s="88"/>
+      <c r="F46" s="6">
+        <v>1001115</v>
+      </c>
+      <c r="G46" s="7">
+        <v>500815</v>
+      </c>
+      <c r="H46" s="7">
+        <v>250781</v>
+      </c>
+      <c r="I46" s="7">
+        <v>167075</v>
+      </c>
+      <c r="J46" s="7">
+        <v>125264</v>
+      </c>
+      <c r="K46" s="7">
+        <v>100245</v>
+      </c>
+      <c r="L46" s="7">
+        <v>83551</v>
+      </c>
+      <c r="M46" s="7">
+        <v>71637</v>
+      </c>
+      <c r="N46" s="7">
+        <v>62698</v>
+      </c>
+      <c r="O46" s="7">
+        <v>55801</v>
+      </c>
+      <c r="P46" s="7">
+        <v>50216</v>
+      </c>
+      <c r="Q46" s="7">
+        <v>45707</v>
+      </c>
+      <c r="R46" s="7">
+        <v>41943</v>
+      </c>
+      <c r="S46" s="7">
+        <v>38650</v>
+      </c>
+      <c r="T46" s="7">
+        <v>35919</v>
+      </c>
+      <c r="U46" s="7">
+        <v>31456</v>
+      </c>
+      <c r="V46" s="7">
+        <v>28023</v>
+      </c>
+      <c r="W46" s="7">
+        <v>25344</v>
+      </c>
+      <c r="X46" s="7">
+        <v>23000</v>
+      </c>
+      <c r="Y46" s="7">
+        <v>21237</v>
+      </c>
+      <c r="Z46" s="7">
+        <v>20191</v>
+      </c>
+      <c r="AA46" s="7">
+        <v>19668</v>
+      </c>
+      <c r="AB46" s="7">
+        <v>18586</v>
+      </c>
+      <c r="AC46" s="7">
+        <v>17709</v>
+      </c>
+      <c r="AD46" s="7">
+        <v>15658</v>
+      </c>
+      <c r="AE46" s="7">
+        <v>13535</v>
+      </c>
+      <c r="AF46" s="7">
+        <v>11975</v>
+      </c>
+      <c r="AG46" s="7">
+        <v>11371</v>
+      </c>
+      <c r="AH46" s="7">
+        <v>10611</v>
+      </c>
+      <c r="AI46" s="7">
+        <v>10018</v>
+      </c>
+      <c r="AJ46" s="7">
+        <v>9497</v>
+      </c>
+      <c r="AK46" s="7">
+        <v>9041</v>
+      </c>
+      <c r="AL46" s="7">
+        <v>8899</v>
+      </c>
+      <c r="AM46" s="127">
+        <v>9081</v>
+      </c>
+      <c r="AN46" s="127">
+        <v>8979</v>
+      </c>
+      <c r="AO46" s="127">
+        <v>9039</v>
+      </c>
+      <c r="AP46" s="127">
+        <v>9078</v>
+      </c>
+      <c r="AQ46" s="127">
+        <v>8944</v>
+      </c>
+      <c r="AR46" s="127">
+        <v>8966</v>
+      </c>
+      <c r="AS46" s="127">
+        <v>9050</v>
+      </c>
+      <c r="AT46" s="127">
+        <v>9040</v>
+      </c>
+      <c r="AU46" s="127">
+        <v>9048</v>
+      </c>
+      <c r="AV46" s="127">
+        <v>9099</v>
+      </c>
+      <c r="AW46" s="127">
+        <v>9081</v>
+      </c>
+      <c r="AX46" s="127">
+        <v>9053</v>
+      </c>
+      <c r="AY46" s="127">
+        <v>9183</v>
+      </c>
+      <c r="AZ46" s="127">
+        <v>9069</v>
+      </c>
+      <c r="BA46" s="128">
+        <v>9198</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="40">
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F40:BA41"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F30:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="C25:C28"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F22:AL23"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F6:AL7"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D8:E9"/>
+    <mergeCell ref="F8:AL9"/>
+    <mergeCell ref="F15:AL16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>